<commit_message>
update mapper reference to branch mapper [50]
</commit_message>
<xml_diff>
--- a/Mapper.xlsx
+++ b/Mapper.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Safrial Wiguna\Documents\GitHub\UNDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEF5362-CBE0-48DD-B311-90F4B80D9B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5AC670-1BB5-4F28-A557-A734E5945533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2355" yWindow="2040" windowWidth="14610" windowHeight="10800" xr2:uid="{7D3D8F4A-0D06-4208-B8F3-CCBACEAC3B04}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7D3D8F4A-0D06-4208-B8F3-CCBACEAC3B04}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapper" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Mapper!$A$1:$M$38</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="78">
   <si>
     <t>Where to Find</t>
   </si>
@@ -245,9 +248,6 @@
     <t>VALIDATE|clinicalStatus-object,coding-array,code-string|active||COMBINENEXT-3</t>
   </si>
   <si>
-    <t>VALIDATE|status-string|completed||COMBINENEXT-2|GET-2-code-coding</t>
-  </si>
-  <si>
     <t>VALIDATE|status-string|completed||COMBINENEXT-3</t>
   </si>
   <si>
@@ -255,6 +255,24 @@
   </si>
   <si>
     <t>VALIDATE|clinicalStatus-object,coding-array,code-string|active||COMBINENEXT-4</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>severity</t>
+  </si>
+  <si>
+    <t>VALIDATE|status-string|final||COMBINENEXT-2</t>
+  </si>
+  <si>
+    <t>COMBINED|GET-code-coding</t>
+  </si>
+  <si>
+    <t>COMBINED|GET-valueCodeableConcept-coding</t>
+  </si>
+  <si>
+    <t>COMBINED|GET-valueString</t>
   </si>
 </sst>
 </file>
@@ -676,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD7AAD0A-388C-4FC3-8829-1D1BBDE3B03B}">
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -793,7 +811,7 @@
         <v>21</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>6</v>
@@ -1038,107 +1056,110 @@
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="2" t="s">
-        <v>38</v>
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>40</v>
+      <c r="H13" t="s">
+        <v>52</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>5</v>
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>72</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>5</v>
+      <c r="H14" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" t="s">
+        <v>54</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
+      </c>
+      <c r="L14" t="s">
+        <v>56</v>
+      </c>
+      <c r="M14" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>25</v>
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>72</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K15" s="2" t="s">
+      <c r="H15" t="s">
+        <v>52</v>
+      </c>
+      <c r="I15" t="s">
+        <v>73</v>
+      </c>
+      <c r="K15" t="s">
         <v>16</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="L15" t="s">
         <v>56</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="M15" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>47</v>
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>72</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>40</v>
+      <c r="H16" t="s">
+        <v>52</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>41</v>
@@ -1146,22 +1167,24 @@
       <c r="K16" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="L16"/>
+      <c r="M16"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>21</v>
@@ -1169,7 +1192,7 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>5</v>
@@ -1184,7 +1207,7 @@
         <v>6</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>5</v>
@@ -1195,7 +1218,7 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>24</v>
@@ -1213,10 +1236,10 @@
         <v>6</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>16</v>
@@ -1230,10 +1253,13 @@
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>45</v>
+        <v>24</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>15</v>
@@ -1245,10 +1271,10 @@
         <v>6</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>15</v>
@@ -1256,27 +1282,27 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="2" customFormat="1">
+    <row r="22" spans="1:13">
       <c r="A22" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>5</v>
@@ -1291,7 +1317,7 @@
         <v>6</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>5</v>
@@ -1302,10 +1328,13 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>50</v>
+        <v>24</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>21</v>
@@ -1317,33 +1346,30 @@
         <v>6</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>16</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>66</v>
@@ -1352,36 +1378,24 @@
         <v>6</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="M24" s="2" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="E25" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>6</v>
@@ -1389,43 +1403,45 @@
       <c r="H25" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="K25" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="2" customFormat="1">
       <c r="A26" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I26" s="4"/>
+        <v>52</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="K26" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>66</v>
@@ -1434,18 +1450,24 @@
         <v>6</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>24</v>
@@ -1463,13 +1485,13 @@
         <v>6</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>56</v>
@@ -1480,37 +1502,42 @@
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="2" t="s">
-        <v>62</v>
+        <v>49</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I29" s="4"/>
+        <v>52</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="K29" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>6</v>
@@ -1518,25 +1545,20 @@
       <c r="H30" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I30" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="I30" s="4"/>
       <c r="K30" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>66</v>
@@ -1548,100 +1570,209 @@
         <v>60</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>40</v>
+        <v>60</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>5</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="I33" s="4"/>
       <c r="K33" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="E36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H34" s="2" t="s">
+      <c r="E38" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="I38" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K34" s="2" t="s">
+      <c r="K38" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L34" s="2" t="s">
+      <c r="L38" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="M34" s="2" t="s">
+      <c r="M38" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
-      <c r="G35" s="3"/>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:M38" xr:uid="{DD7AAD0A-388C-4FC3-8829-1D1BBDE3B03B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
@@ -1657,14 +1788,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="dab150e2-07c8-46cb-9249-a9bf8b457629" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A6BA5F8C2D628444819C98CC51374019" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d1ade1ff80079ef11d5f7598ff2bdcd2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dab150e2-07c8-46cb-9249-a9bf8b457629" xmlns:ns4="3b2a6cf9-543e-463e-8642-d16a96cd5df5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="604d7b76327a76c6db5227909a871758" ns3:_="" ns4:_="">
     <xsd:import namespace="dab150e2-07c8-46cb-9249-a9bf8b457629"/>
@@ -1891,6 +2014,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="dab150e2-07c8-46cb-9249-a9bf8b457629" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A52368F7-EAC7-45FB-9A71-35E9ACE10DED}">
   <ds:schemaRefs>
@@ -1900,23 +2031,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41D37996-5A98-4323-941F-5BAF649EAAF0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3b2a6cf9-543e-463e-8642-d16a96cd5df5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="dab150e2-07c8-46cb-9249-a9bf8b457629"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE9DBFBC-8664-4C0E-9CBF-BAF1CF3B6304}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1933,4 +2047,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41D37996-5A98-4323-941F-5BAF649EAAF0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3b2a6cf9-543e-463e-8642-d16a96cd5df5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="dab150e2-07c8-46cb-9249-a9bf8b457629"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update if id not found
</commit_message>
<xml_diff>
--- a/Mapper.xlsx
+++ b/Mapper.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Safrial Wiguna\Documents\GitHub\UNDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5AC670-1BB5-4F28-A557-A734E5945533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE09DCB-BD14-4AEF-AB30-ED4393D618E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7D3D8F4A-0D06-4208-B8F3-CCBACEAC3B04}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapper" sheetId="1" r:id="rId1"/>
+    <sheet name="Lembar1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Mapper!$A$1:$M$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Mapper!$A$1:$M$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="89">
   <si>
     <t>Where to Find</t>
   </si>
@@ -273,6 +274,39 @@
   </si>
   <si>
     <t>COMBINED|GET-valueString</t>
+  </si>
+  <si>
+    <t>medicationReference</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>COMBINED|GETREF-code-coding</t>
+  </si>
+  <si>
+    <t>MedicationRequest/MedicationDispense</t>
+  </si>
+  <si>
+    <t>VALIDATE|status-string|activeORcompleted||COMBINENEXT-4</t>
+  </si>
+  <si>
+    <t>dosageInstruction</t>
+  </si>
+  <si>
+    <t>routeOfAdministration</t>
+  </si>
+  <si>
+    <t>COMBINED|GET-route-coding</t>
+  </si>
+  <si>
+    <t>COMBINED|GET-doseAndRate-doseQuantity</t>
+  </si>
+  <si>
+    <t>doseIntervals</t>
+  </si>
+  <si>
+    <t>quantity</t>
   </si>
 </sst>
 </file>
@@ -694,15 +728,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD7AAD0A-388C-4FC3-8829-1D1BBDE3B03B}">
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
@@ -1531,7 +1565,7 @@
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>21</v>
@@ -1543,16 +1577,15 @@
         <v>6</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I30" s="4"/>
+        <v>40</v>
+      </c>
       <c r="K30" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>5</v>
@@ -1567,7 +1600,7 @@
         <v>6</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>5</v>
@@ -1578,28 +1611,25 @@
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>16</v>
@@ -1608,166 +1638,6 @@
         <v>56</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13">
-      <c r="A33" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I33" s="4"/>
-      <c r="K33" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13">
-      <c r="A34" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13">
-      <c r="A35" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L35" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="M35" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13">
-      <c r="A38" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="M38" s="2" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1775,6 +1645,384 @@
   <autoFilter ref="A1:M38" xr:uid="{DD7AAD0A-388C-4FC3-8829-1D1BBDE3B03B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE0E3FA-A925-4575-A763-7625F13D8F40}">
+  <dimension ref="A1:M12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="4"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" t="s">
+        <v>84</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L11" t="s">
+        <v>56</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I12" t="s">
+        <v>87</v>
+      </c>
+      <c r="J12" t="s">
+        <v>88</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12" t="s">
+        <v>58</v>
+      </c>
+      <c r="M12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1788,6 +2036,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="dab150e2-07c8-46cb-9249-a9bf8b457629" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A6BA5F8C2D628444819C98CC51374019" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d1ade1ff80079ef11d5f7598ff2bdcd2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dab150e2-07c8-46cb-9249-a9bf8b457629" xmlns:ns4="3b2a6cf9-543e-463e-8642-d16a96cd5df5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="604d7b76327a76c6db5227909a871758" ns3:_="" ns4:_="">
     <xsd:import namespace="dab150e2-07c8-46cb-9249-a9bf8b457629"/>
@@ -2014,14 +2270,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="dab150e2-07c8-46cb-9249-a9bf8b457629" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A52368F7-EAC7-45FB-9A71-35E9ACE10DED}">
   <ds:schemaRefs>
@@ -2031,6 +2279,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41D37996-5A98-4323-941F-5BAF649EAAF0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3b2a6cf9-543e-463e-8642-d16a96cd5df5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="dab150e2-07c8-46cb-9249-a9bf8b457629"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE9DBFBC-8664-4C0E-9CBF-BAF1CF3B6304}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2047,21 +2312,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41D37996-5A98-4323-941F-5BAF649EAAF0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3b2a6cf9-543e-463e-8642-d16a96cd5df5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="dab150e2-07c8-46cb-9249-a9bf8b457629"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update mapper && prepare validation
</commit_message>
<xml_diff>
--- a/Mapper.xlsx
+++ b/Mapper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Safrial Wiguna\Documents\GitHub\UNDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE09DCB-BD14-4AEF-AB30-ED4393D618E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17E6539-2EDB-409D-A88C-64CE9992837E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7D3D8F4A-0D06-4208-B8F3-CCBACEAC3B04}"/>
   </bookViews>
@@ -264,9 +264,6 @@
     <t>severity</t>
   </si>
   <si>
-    <t>VALIDATE|status-string|final||COMBINENEXT-2</t>
-  </si>
-  <si>
     <t>COMBINED|GET-code-coding</t>
   </si>
   <si>
@@ -288,9 +285,6 @@
     <t>MedicationRequest/MedicationDispense</t>
   </si>
   <si>
-    <t>VALIDATE|status-string|activeORcompleted||COMBINENEXT-4</t>
-  </si>
-  <si>
     <t>dosageInstruction</t>
   </si>
   <si>
@@ -307,6 +301,12 @@
   </si>
   <si>
     <t>quantity</t>
+  </si>
+  <si>
+    <t>VALIDATE|status-string|final||COMBINENEXT-3</t>
+  </si>
+  <si>
+    <t>VALIDATE|status-string|activeORcompleted||COMBINENEXT-4-MedicationDispense||COMBINENEXT-2-MedicationRequest</t>
   </si>
 </sst>
 </file>
@@ -728,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD7AAD0A-388C-4FC3-8829-1D1BBDE3B03B}">
-  <dimension ref="A1:M32"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="D28" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -740,10 +740,10 @@
     <col min="2" max="2" width="27" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="75.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="111.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="69" style="2" bestFit="1" customWidth="1"/>
@@ -1100,7 +1100,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>6</v>
@@ -1123,7 +1123,7 @@
         <v>21</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>6</v>
@@ -1155,7 +1155,7 @@
         <v>21</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>6</v>
@@ -1187,7 +1187,7 @@
         <v>21</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>6</v>
@@ -1620,7 +1620,7 @@
         <v>21</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>6</v>
@@ -1638,6 +1638,163 @@
         <v>56</v>
       </c>
       <c r="M32" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I36" t="s">
+        <v>82</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L36" t="s">
+        <v>56</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I37" t="s">
+        <v>85</v>
+      </c>
+      <c r="J37" t="s">
+        <v>86</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L37" t="s">
+        <v>58</v>
+      </c>
+      <c r="M37" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1650,10 +1807,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE0E3FA-A925-4575-A763-7625F13D8F40}">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A8" sqref="A8:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1848,199 +2005,26 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I11" t="s">
-        <v>84</v>
-      </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L11" t="s">
-        <v>56</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I12" t="s">
-        <v>87</v>
-      </c>
-      <c r="J12" t="s">
-        <v>88</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L12" t="s">
-        <v>58</v>
-      </c>
-      <c r="M12" t="s">
-        <v>48</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="dab150e2-07c8-46cb-9249-a9bf8b457629" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="dab150e2-07c8-46cb-9249-a9bf8b457629" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2271,14 +2255,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A52368F7-EAC7-45FB-9A71-35E9ACE10DED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41D37996-5A98-4323-941F-5BAF649EAAF0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2291,6 +2267,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A52368F7-EAC7-45FB-9A71-35E9ACE10DED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
mapper adjustment for observation.component
</commit_message>
<xml_diff>
--- a/Mapper.xlsx
+++ b/Mapper.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -604,10 +604,10 @@
         <v>Observation</v>
       </c>
       <c r="B8" t="str">
-        <v>valueString</v>
+        <v>valueQuantity</v>
       </c>
       <c r="E8" t="str">
-        <v>string</v>
+        <v>object</v>
       </c>
       <c r="F8" t="str">
         <v>COMBINED</v>
@@ -619,10 +619,16 @@
         <v>measurements</v>
       </c>
       <c r="I8" t="str">
-        <v>notes</v>
+        <v>measurementValue</v>
       </c>
       <c r="K8" t="str">
-        <v>string</v>
+        <v>object</v>
+      </c>
+      <c r="L8" t="str">
+        <v>TRANSFORM-unit[id:label],value|Value-system,code-[unitcode:code],value</v>
+      </c>
+      <c r="M8" t="str">
+        <v>[{"system":"http://snomed.info/sct","code":"SNOMED"},{"system":"http://loinc.org","code":"LOINC"},{"system":"http://unitsofmeasure.org","code":"UCUM"},{"system":"http://terminology.hl7.org/CodeSystem/condition-category","code":"HL7"},{"system":"http://hl7.org/fhir/sid/icd-10","code":"ICD10"},{"system":"http://www.whocc.no/atc","code":"WHO"},{"system":"http://terminology.kemkes.go.id/CodeSystem/clinical-term","code":"KEMKES"},{"system":"http://sys-ids.kemkes.go.id/kfa","code":"KFA"},{"system":"http://hl7.org/fhir/sid/icd-9-cm","code":"ICD9CM"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-topography","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-morphology","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-t-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-n-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-m-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/examination","code":"KEMKES"}]</v>
       </c>
     </row>
     <row r="9">
@@ -630,10 +636,10 @@
         <v>Observation</v>
       </c>
       <c r="B9" t="str">
-        <v>valueQuantity</v>
+        <v>valueInteger</v>
       </c>
       <c r="E9" t="str">
-        <v>object</v>
+        <v>number</v>
       </c>
       <c r="F9" t="str">
         <v>COMBINED</v>
@@ -648,13 +654,7 @@
         <v>measurementValue</v>
       </c>
       <c r="K9" t="str">
-        <v>object</v>
-      </c>
-      <c r="L9" t="str">
-        <v>TRANSFORM-unit[id:label],value|Value-system,code-[unitcode:code],value</v>
-      </c>
-      <c r="M9" t="str">
-        <v>[{"system":"http://snomed.info/sct","code":"SNOMED"},{"system":"http://loinc.org","code":"LOINC"},{"system":"http://unitsofmeasure.org","code":"UCUM"},{"system":"http://terminology.hl7.org/CodeSystem/condition-category","code":"HL7"},{"system":"http://hl7.org/fhir/sid/icd-10","code":"ICD10"},{"system":"http://www.whocc.no/atc","code":"WHO"},{"system":"http://terminology.kemkes.go.id/CodeSystem/clinical-term","code":"KEMKES"},{"system":"http://sys-ids.kemkes.go.id/kfa","code":"KFA"},{"system":"http://hl7.org/fhir/sid/icd-9-cm","code":"ICD9CM"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-topography","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-morphology","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-t-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-n-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-m-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/examination","code":"KEMKES"}]</v>
+        <v>number</v>
       </c>
     </row>
     <row r="10">
@@ -662,13 +662,10 @@
         <v>Observation</v>
       </c>
       <c r="B10" t="str">
-        <v>valueCodeableConcept</v>
-      </c>
-      <c r="C10" t="str">
-        <v>coding</v>
+        <v>effectiveDateTime</v>
       </c>
       <c r="E10" t="str">
-        <v>array</v>
+        <v>string</v>
       </c>
       <c r="F10" t="str">
         <v>COMBINED</v>
@@ -680,16 +677,10 @@
         <v>measurements</v>
       </c>
       <c r="I10" t="str">
-        <v>measurementValue</v>
+        <v>date</v>
       </c>
       <c r="K10" t="str">
-        <v>object</v>
-      </c>
-      <c r="L10" t="str">
-        <v>TRANSFORM-unit[id:label]|Value-system,code-[unitcode:display]</v>
-      </c>
-      <c r="M10" t="str">
-        <v>[{"system":"http://snomed.info/sct","code":"SNOMED"},{"system":"http://loinc.org","code":"LOINC"},{"system":"http://unitsofmeasure.org","code":"UCUM"},{"system":"http://terminology.hl7.org/CodeSystem/condition-category","code":"HL7"},{"system":"http://hl7.org/fhir/sid/icd-10","code":"ICD10"},{"system":"http://www.whocc.no/atc","code":"WHO"},{"system":"http://terminology.kemkes.go.id/CodeSystem/clinical-term","code":"KEMKES"},{"system":"http://sys-ids.kemkes.go.id/kfa","code":"KFA"},{"system":"http://hl7.org/fhir/sid/icd-9-cm","code":"ICD9CM"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-topography","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-morphology","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-t-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-n-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-m-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/examination","code":"KEMKES"}]</v>
+        <v>string</v>
       </c>
     </row>
     <row r="11">
@@ -697,25 +688,25 @@
         <v>Observation</v>
       </c>
       <c r="B11" t="str">
-        <v>valueInteger</v>
+        <v>component</v>
+      </c>
+      <c r="C11" t="str">
+        <v>coding</v>
       </c>
       <c r="E11" t="str">
-        <v>number</v>
+        <v>array</v>
       </c>
       <c r="F11" t="str">
-        <v>COMBINED</v>
+        <v>VALIDATE|NOT-code-coding-system-string|http://snomed.info/sct|COMBINENEXT-8</v>
       </c>
       <c r="G11" t="str">
         <v>individuals</v>
       </c>
       <c r="H11" t="str">
-        <v>measurements</v>
-      </c>
-      <c r="I11" t="str">
-        <v>measurementValue</v>
+        <v>phenotypicFeatures</v>
       </c>
       <c r="K11" t="str">
-        <v>number</v>
+        <v>array</v>
       </c>
     </row>
     <row r="12">
@@ -723,25 +714,28 @@
         <v>Observation</v>
       </c>
       <c r="B12" t="str">
-        <v>effectiveDateTime</v>
+        <v>component</v>
+      </c>
+      <c r="C12" t="str">
+        <v>valueBoolean</v>
       </c>
       <c r="E12" t="str">
-        <v>string</v>
+        <v>boolean</v>
       </c>
       <c r="F12" t="str">
-        <v>COMBINED</v>
+        <v>VALIDATE|valueBoolean|true|COMBINENEXT-7</v>
       </c>
       <c r="G12" t="str">
         <v>individuals</v>
       </c>
       <c r="H12" t="str">
-        <v>measurements</v>
+        <v>phenotypicFeatures</v>
       </c>
       <c r="I12" t="str">
-        <v>date</v>
+        <v>excluded</v>
       </c>
       <c r="K12" t="str">
-        <v>string</v>
+        <v>boolean</v>
       </c>
     </row>
     <row r="13">
@@ -749,13 +743,16 @@
         <v>Observation</v>
       </c>
       <c r="B13" t="str">
-        <v>component</v>
+        <v>code</v>
+      </c>
+      <c r="C13" t="str">
+        <v>coding</v>
       </c>
       <c r="E13" t="str">
         <v>array</v>
       </c>
       <c r="F13" t="str">
-        <v>VALIDATE|COMBINENEXT-5</v>
+        <v>COMBINED</v>
       </c>
       <c r="G13" t="str">
         <v>individuals</v>
@@ -763,8 +760,17 @@
       <c r="H13" t="str">
         <v>phenotypicFeatures</v>
       </c>
+      <c r="I13" t="str">
+        <v>featureType</v>
+      </c>
       <c r="K13" t="str">
-        <v>array</v>
+        <v>object</v>
+      </c>
+      <c r="L13" t="str">
+        <v>TRANSFORM-id,label|Default Value-type-code,value</v>
+      </c>
+      <c r="M13" t="str">
+        <v>[{"type":"environment","code":"SNOMED:414285001","value":"Allergy to substance (disorder)"},{"type":"medication","code":"SNOMED:416098002","value":"Drug allergy (disorder)"},{"type":"food","code":"SNOMED:426232007","value":"Allergy to food (disorder)"},{"type":"biologic","code":"FHIR:biologic","value":"Biologic"}]</v>
       </c>
     </row>
     <row r="14">
@@ -775,13 +781,16 @@
         <v>component</v>
       </c>
       <c r="C14" t="str">
-        <v>valueBoolean</v>
+        <v>code</v>
+      </c>
+      <c r="D14" t="str">
+        <v>coding</v>
       </c>
       <c r="E14" t="str">
-        <v>boolean</v>
+        <v>array</v>
       </c>
       <c r="F14" t="str">
-        <v>VALIDATE|valueBoolean|true|COMBINENEXT-4</v>
+        <v>COMBINED</v>
       </c>
       <c r="G14" t="str">
         <v>individuals</v>
@@ -790,10 +799,19 @@
         <v>phenotypicFeatures</v>
       </c>
       <c r="I14" t="str">
-        <v>excluded</v>
+        <v>featureType</v>
+      </c>
+      <c r="J14" t="str">
+        <v>modifiers</v>
       </c>
       <c r="K14" t="str">
-        <v>boolean</v>
+        <v>array</v>
+      </c>
+      <c r="L14" t="str">
+        <v>TRANSFORM-id,label|Coding-system,code-unitcode,display</v>
+      </c>
+      <c r="M14" t="str">
+        <v>[{"system":"http://snomed.info/sct","code":"SNOMED"},{"system":"http://loinc.org","code":"LOINC"},{"system":"http://unitsofmeasure.org","code":"UCUM"},{"system":"http://terminology.hl7.org/CodeSystem/condition-category","code":"HL7"},{"system":"http://hl7.org/fhir/sid/icd-10","code":"ICD10"},{"system":"http://www.whocc.no/atc","code":"WHO"},{"system":"http://terminology.kemkes.go.id/CodeSystem/clinical-term","code":"KEMKES"},{"system":"http://sys-ids.kemkes.go.id/kfa","code":"KFA"},{"system":"http://hl7.org/fhir/sid/icd-9-cm","code":"ICD9CM"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-topography","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-morphology","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-t-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-n-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-m-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/examination","code":"KEMKES"}]</v>
       </c>
     </row>
     <row r="15">
@@ -801,9 +819,12 @@
         <v>Observation</v>
       </c>
       <c r="B15" t="str">
-        <v>code</v>
+        <v>component</v>
       </c>
       <c r="C15" t="str">
+        <v>valueCodeableConcept</v>
+      </c>
+      <c r="D15" t="str">
         <v>coding</v>
       </c>
       <c r="E15" t="str">
@@ -821,14 +842,14 @@
       <c r="I15" t="str">
         <v>featureType</v>
       </c>
+      <c r="J15" t="str">
+        <v>severity</v>
+      </c>
       <c r="K15" t="str">
         <v>object</v>
       </c>
       <c r="L15" t="str">
-        <v>TRANSFORM-id,label|Default Value-type-code,value</v>
-      </c>
-      <c r="M15" t="str">
-        <v>[{"type":"environment","code":"SNOMED:414285001","value":"Allergy to substance (disorder)"},{"type":"medication","code":"SNOMED:416098002","value":"Drug allergy (disorder)"},{"type":"food","code":"SNOMED:426232007","value":"Allergy to food (disorder)"},{"type":"biologic","code":"FHIR:biologic","value":"Biologic"}]</v>
+        <v>TRANSFORM-id,label|Coding-system,code-unitcode,display</v>
       </c>
     </row>
     <row r="16">
@@ -839,13 +860,10 @@
         <v>component</v>
       </c>
       <c r="C16" t="str">
-        <v>code</v>
-      </c>
-      <c r="D16" t="str">
-        <v>coding</v>
+        <v>valueString</v>
       </c>
       <c r="E16" t="str">
-        <v>array</v>
+        <v>string</v>
       </c>
       <c r="F16" t="str">
         <v>COMBINED</v>
@@ -857,19 +875,10 @@
         <v>phenotypicFeatures</v>
       </c>
       <c r="I16" t="str">
-        <v>featureType</v>
-      </c>
-      <c r="J16" t="str">
-        <v>modifiers</v>
+        <v>notes</v>
       </c>
       <c r="K16" t="str">
-        <v>array</v>
-      </c>
-      <c r="L16" t="str">
-        <v>TRANSFORM-id,label|Coding-system,code-unitcode,display</v>
-      </c>
-      <c r="M16" t="str">
-        <v>[{"system":"http://snomed.info/sct","code":"SNOMED"},{"system":"http://loinc.org","code":"LOINC"},{"system":"http://unitsofmeasure.org","code":"UCUM"},{"system":"http://terminology.hl7.org/CodeSystem/condition-category","code":"HL7"},{"system":"http://hl7.org/fhir/sid/icd-10","code":"ICD10"},{"system":"http://www.whocc.no/atc","code":"WHO"},{"system":"http://terminology.kemkes.go.id/CodeSystem/clinical-term","code":"KEMKES"},{"system":"http://sys-ids.kemkes.go.id/kfa","code":"KFA"},{"system":"http://hl7.org/fhir/sid/icd-9-cm","code":"ICD9CM"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-topography","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-morphology","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-t-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-n-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-m-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/examination","code":"KEMKES"}]</v>
+        <v>string</v>
       </c>
     </row>
     <row r="17">
@@ -880,34 +889,19 @@
         <v>component</v>
       </c>
       <c r="C17" t="str">
-        <v>valueCodeableConcept</v>
-      </c>
-      <c r="D17" t="str">
         <v>coding</v>
       </c>
       <c r="E17" t="str">
         <v>array</v>
       </c>
       <c r="F17" t="str">
-        <v>COMBINED</v>
+        <v>VALIDATE|code-coding-system-string|http://snomed.info/sct|COMBINENEXT-2</v>
       </c>
       <c r="G17" t="str">
         <v>individuals</v>
       </c>
       <c r="H17" t="str">
-        <v>phenotypicFeatures</v>
-      </c>
-      <c r="I17" t="str">
-        <v>featureType</v>
-      </c>
-      <c r="J17" t="str">
-        <v>severity</v>
-      </c>
-      <c r="K17" t="str">
-        <v>object</v>
-      </c>
-      <c r="L17" t="str">
-        <v>TRANSFORM-id,label|Coding-system,code-unitcode,display</v>
+        <v>diseases</v>
       </c>
     </row>
     <row r="18">
@@ -918,10 +912,10 @@
         <v>component</v>
       </c>
       <c r="C18" t="str">
-        <v>valueString</v>
+        <v>coding</v>
       </c>
       <c r="E18" t="str">
-        <v>string</v>
+        <v>array</v>
       </c>
       <c r="F18" t="str">
         <v>COMBINED</v>
@@ -930,50 +924,38 @@
         <v>individuals</v>
       </c>
       <c r="H18" t="str">
-        <v>phenotypicFeatures</v>
+        <v>diseases</v>
       </c>
       <c r="I18" t="str">
-        <v>notes</v>
+        <v>diseaseCode</v>
       </c>
       <c r="K18" t="str">
-        <v>string</v>
+        <v>object</v>
+      </c>
+      <c r="L18" t="str">
+        <v>TRANSFORM-id,label|Coding-system,code-unitcode,display</v>
+      </c>
+      <c r="M18" t="str">
+        <v>[{"system":"http://snomed.info/sct","code":"SNOMED"},{"system":"http://loinc.org","code":"LOINC"},{"system":"http://unitsofmeasure.org","code":"UCUM"},{"system":"http://terminology.hl7.org/CodeSystem/condition-category","code":"HL7"},{"system":"http://hl7.org/fhir/sid/icd-10","code":"ICD10"},{"system":"http://www.whocc.no/atc","code":"WHO"},{"system":"http://terminology.kemkes.go.id/CodeSystem/clinical-term","code":"KEMKES"},{"system":"http://sys-ids.kemkes.go.id/kfa","code":"KFA"},{"system":"http://hl7.org/fhir/sid/icd-9-cm","code":"ICD9CM"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-topography","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-morphology","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-t-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-n-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-m-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/examination","code":"KEMKES"}]</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>Condition</v>
-      </c>
-      <c r="E19" t="str">
-        <v>array</v>
-      </c>
-      <c r="F19" t="str">
-        <v>VALIDATE|clinicalStatus-object,coding-array,code-string|active||COMBINENEXT-3</v>
-      </c>
-      <c r="G19" t="str">
-        <v>individuals</v>
-      </c>
-      <c r="H19" t="str">
-        <v>diseases</v>
-      </c>
-      <c r="K19" t="str">
-        <v>array</v>
+        <v>Observation</v>
+      </c>
+      <c r="B19" t="str">
+        <v>component</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
         <v>Condition</v>
       </c>
-      <c r="B20" t="str">
-        <v>subject</v>
-      </c>
-      <c r="C20" t="str">
-        <v>reference</v>
-      </c>
       <c r="E20" t="str">
-        <v>string</v>
+        <v>array</v>
       </c>
       <c r="F20" t="str">
-        <v>COMBINED</v>
+        <v>VALIDATE|clinicalStatus-object,coding-array,code-string|active||COMBINENEXT-3</v>
       </c>
       <c r="G20" t="str">
         <v>individuals</v>
@@ -981,14 +963,8 @@
       <c r="H20" t="str">
         <v>diseases</v>
       </c>
-      <c r="I20" t="str">
-        <v>id</v>
-      </c>
       <c r="K20" t="str">
-        <v>string</v>
-      </c>
-      <c r="L20" t="str">
-        <v>TRANSFORM-id|SPLIT(/,-1)</v>
+        <v>array</v>
       </c>
     </row>
     <row r="21">
@@ -996,13 +972,13 @@
         <v>Condition</v>
       </c>
       <c r="B21" t="str">
-        <v>code</v>
+        <v>subject</v>
       </c>
       <c r="C21" t="str">
-        <v>coding</v>
+        <v>reference</v>
       </c>
       <c r="E21" t="str">
-        <v>array</v>
+        <v>string</v>
       </c>
       <c r="F21" t="str">
         <v>COMBINED</v>
@@ -1014,16 +990,13 @@
         <v>diseases</v>
       </c>
       <c r="I21" t="str">
-        <v>diseaseCode</v>
+        <v>id</v>
       </c>
       <c r="K21" t="str">
-        <v>object</v>
+        <v>string</v>
       </c>
       <c r="L21" t="str">
-        <v>TRANSFORM-id,label|Coding-system,code-unitcode,display</v>
-      </c>
-      <c r="M21" t="str">
-        <v>[{"system":"http://snomed.info/sct","code":"SNOMED"},{"system":"http://loinc.org","code":"LOINC"},{"system":"http://unitsofmeasure.org","code":"UCUM"},{"system":"http://terminology.hl7.org/CodeSystem/condition-category","code":"HL7"},{"system":"http://hl7.org/fhir/sid/icd-10","code":"ICD10"},{"system":"http://www.whocc.no/atc","code":"WHO"},{"system":"http://terminology.kemkes.go.id/CodeSystem/clinical-term","code":"KEMKES"},{"system":"http://sys-ids.kemkes.go.id/kfa","code":"KFA"},{"system":"http://hl7.org/fhir/sid/icd-9-cm","code":"ICD9CM"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-topography","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-morphology","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-t-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-n-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-m-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/examination","code":"KEMKES"}]</v>
+        <v>TRANSFORM-id|SPLIT(/,-1)</v>
       </c>
     </row>
     <row r="22">
@@ -1034,10 +1007,10 @@
         <v>code</v>
       </c>
       <c r="C22" t="str">
-        <v>text</v>
+        <v>coding</v>
       </c>
       <c r="E22" t="str">
-        <v>string</v>
+        <v>array</v>
       </c>
       <c r="F22" t="str">
         <v>COMBINED</v>
@@ -1049,47 +1022,56 @@
         <v>diseases</v>
       </c>
       <c r="I22" t="str">
-        <v>notes</v>
+        <v>diseaseCode</v>
       </c>
       <c r="K22" t="str">
-        <v>string</v>
+        <v>object</v>
+      </c>
+      <c r="L22" t="str">
+        <v>TRANSFORM-id,label|Coding-system,code-unitcode,display</v>
+      </c>
+      <c r="M22" t="str">
+        <v>[{"system":"http://snomed.info/sct","code":"SNOMED"},{"system":"http://loinc.org","code":"LOINC"},{"system":"http://unitsofmeasure.org","code":"UCUM"},{"system":"http://terminology.hl7.org/CodeSystem/condition-category","code":"HL7"},{"system":"http://hl7.org/fhir/sid/icd-10","code":"ICD10"},{"system":"http://www.whocc.no/atc","code":"WHO"},{"system":"http://terminology.kemkes.go.id/CodeSystem/clinical-term","code":"KEMKES"},{"system":"http://sys-ids.kemkes.go.id/kfa","code":"KFA"},{"system":"http://hl7.org/fhir/sid/icd-9-cm","code":"ICD9CM"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-topography","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-morphology","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-t-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-n-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-m-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/examination","code":"KEMKES"}]</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>Procedure</v>
+        <v>Condition</v>
+      </c>
+      <c r="B23" t="str">
+        <v>code</v>
+      </c>
+      <c r="C23" t="str">
+        <v>text</v>
       </c>
       <c r="E23" t="str">
-        <v>array</v>
+        <v>string</v>
       </c>
       <c r="F23" t="str">
-        <v>VALIDATE|status-string|completed||COMBINENEXT-3</v>
+        <v>COMBINED</v>
       </c>
       <c r="G23" t="str">
         <v>individuals</v>
       </c>
       <c r="H23" t="str">
-        <v>interventionsOrProcedures</v>
+        <v>diseases</v>
+      </c>
+      <c r="I23" t="str">
+        <v>notes</v>
       </c>
       <c r="K23" t="str">
-        <v>array</v>
+        <v>string</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
         <v>Procedure</v>
       </c>
-      <c r="B24" t="str">
-        <v>subject</v>
-      </c>
-      <c r="C24" t="str">
-        <v>reference</v>
-      </c>
       <c r="E24" t="str">
-        <v>string</v>
+        <v>array</v>
       </c>
       <c r="F24" t="str">
-        <v>COMBINED</v>
+        <v>VALIDATE|status-string|completed||COMBINENEXT-3</v>
       </c>
       <c r="G24" t="str">
         <v>individuals</v>
@@ -1097,14 +1079,8 @@
       <c r="H24" t="str">
         <v>interventionsOrProcedures</v>
       </c>
-      <c r="I24" t="str">
-        <v>id</v>
-      </c>
       <c r="K24" t="str">
-        <v>string</v>
-      </c>
-      <c r="L24" t="str">
-        <v>TRANSFORM-id|SPLIT(/,-1)</v>
+        <v>array</v>
       </c>
     </row>
     <row r="25">
@@ -1112,13 +1088,13 @@
         <v>Procedure</v>
       </c>
       <c r="B25" t="str">
-        <v>code</v>
+        <v>subject</v>
       </c>
       <c r="C25" t="str">
-        <v>coding</v>
+        <v>reference</v>
       </c>
       <c r="E25" t="str">
-        <v>array</v>
+        <v>string</v>
       </c>
       <c r="F25" t="str">
         <v>COMBINED</v>
@@ -1130,16 +1106,13 @@
         <v>interventionsOrProcedures</v>
       </c>
       <c r="I25" t="str">
-        <v>procedureCode</v>
+        <v>id</v>
       </c>
       <c r="K25" t="str">
-        <v>object</v>
+        <v>string</v>
       </c>
       <c r="L25" t="str">
-        <v>TRANSFORM-id,label|Coding-system,code-unitcode,display</v>
-      </c>
-      <c r="M25" t="str">
-        <v>[{"system":"http://snomed.info/sct","code":"SNOMED"},{"system":"http://loinc.org","code":"LOINC"},{"system":"http://unitsofmeasure.org","code":"UCUM"},{"system":"http://terminology.hl7.org/CodeSystem/condition-category","code":"HL7"},{"system":"http://hl7.org/fhir/sid/icd-10","code":"ICD10"},{"system":"http://www.whocc.no/atc","code":"WHO"},{"system":"http://terminology.kemkes.go.id/CodeSystem/clinical-term","code":"KEMKES"},{"system":"http://sys-ids.kemkes.go.id/kfa","code":"KFA"},{"system":"http://hl7.org/fhir/sid/icd-9-cm","code":"ICD9CM"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-topography","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-morphology","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-t-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-n-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-m-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/examination","code":"KEMKES"}]</v>
+        <v>TRANSFORM-id|SPLIT(/,-1)</v>
       </c>
     </row>
     <row r="26">
@@ -1147,10 +1120,13 @@
         <v>Procedure</v>
       </c>
       <c r="B26" t="str">
-        <v>performedDateTime</v>
+        <v>code</v>
+      </c>
+      <c r="C26" t="str">
+        <v>coding</v>
       </c>
       <c r="E26" t="str">
-        <v>string</v>
+        <v>array</v>
       </c>
       <c r="F26" t="str">
         <v>COMBINED</v>
@@ -1162,47 +1138,53 @@
         <v>interventionsOrProcedures</v>
       </c>
       <c r="I26" t="str">
-        <v>dateOfProcedure</v>
+        <v>procedureCode</v>
       </c>
       <c r="K26" t="str">
-        <v>string</v>
+        <v>object</v>
+      </c>
+      <c r="L26" t="str">
+        <v>TRANSFORM-id,label|Coding-system,code-unitcode,display</v>
+      </c>
+      <c r="M26" t="str">
+        <v>[{"system":"http://snomed.info/sct","code":"SNOMED"},{"system":"http://loinc.org","code":"LOINC"},{"system":"http://unitsofmeasure.org","code":"UCUM"},{"system":"http://terminology.hl7.org/CodeSystem/condition-category","code":"HL7"},{"system":"http://hl7.org/fhir/sid/icd-10","code":"ICD10"},{"system":"http://www.whocc.no/atc","code":"WHO"},{"system":"http://terminology.kemkes.go.id/CodeSystem/clinical-term","code":"KEMKES"},{"system":"http://sys-ids.kemkes.go.id/kfa","code":"KFA"},{"system":"http://hl7.org/fhir/sid/icd-9-cm","code":"ICD9CM"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-topography","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-morphology","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-t-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-n-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-m-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/examination","code":"KEMKES"}]</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>AllergyIntolerance</v>
+        <v>Procedure</v>
+      </c>
+      <c r="B27" t="str">
+        <v>performedDateTime</v>
       </c>
       <c r="E27" t="str">
-        <v>array</v>
+        <v>string</v>
       </c>
       <c r="F27" t="str">
-        <v>VALIDATE|clinicalStatus-object,coding-array,code-string|active||COMBINENEXT-4</v>
+        <v>COMBINED</v>
       </c>
       <c r="G27" t="str">
         <v>individuals</v>
       </c>
       <c r="H27" t="str">
-        <v>phenotypicFeatures</v>
+        <v>interventionsOrProcedures</v>
+      </c>
+      <c r="I27" t="str">
+        <v>dateOfProcedure</v>
       </c>
       <c r="K27" t="str">
-        <v>array</v>
+        <v>string</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
         <v>AllergyIntolerance</v>
       </c>
-      <c r="B28" t="str">
-        <v>patient</v>
-      </c>
-      <c r="C28" t="str">
-        <v>reference</v>
-      </c>
       <c r="E28" t="str">
-        <v>string</v>
+        <v>array</v>
       </c>
       <c r="F28" t="str">
-        <v>COMBINED</v>
+        <v>VALIDATE|clinicalStatus-object,coding-array,code-string|active||COMBINENEXT-4</v>
       </c>
       <c r="G28" t="str">
         <v>individuals</v>
@@ -1210,14 +1192,8 @@
       <c r="H28" t="str">
         <v>phenotypicFeatures</v>
       </c>
-      <c r="I28" t="str">
-        <v>id</v>
-      </c>
       <c r="K28" t="str">
-        <v>string</v>
-      </c>
-      <c r="L28" t="str">
-        <v>TRANSFORM-id|SPLIT(/,-1)</v>
+        <v>array</v>
       </c>
     </row>
     <row r="29">
@@ -1225,10 +1201,13 @@
         <v>AllergyIntolerance</v>
       </c>
       <c r="B29" t="str">
-        <v>category</v>
+        <v>patient</v>
+      </c>
+      <c r="C29" t="str">
+        <v>reference</v>
       </c>
       <c r="E29" t="str">
-        <v>array</v>
+        <v>string</v>
       </c>
       <c r="F29" t="str">
         <v>COMBINED</v>
@@ -1240,16 +1219,13 @@
         <v>phenotypicFeatures</v>
       </c>
       <c r="I29" t="str">
-        <v>featureType</v>
+        <v>id</v>
       </c>
       <c r="K29" t="str">
-        <v>object</v>
+        <v>string</v>
       </c>
       <c r="L29" t="str">
-        <v>TRANSFORM-id,label|Default Value-type-code,value</v>
-      </c>
-      <c r="M29" t="str">
-        <v>[{"type":"environment","code":"SNOMED:414285001","value":"Allergy to substance (disorder)"},{"type":"medication","code":"SNOMED:416098002","value":"Drug allergy (disorder)"},{"type":"food","code":"SNOMED:426232007","value":"Allergy to food (disorder)"},{"type":"biologic","code":"FHIR:biologic","value":"Biologic"}]</v>
+        <v>TRANSFORM-id|SPLIT(/,-1)</v>
       </c>
     </row>
     <row r="30">
@@ -1257,10 +1233,7 @@
         <v>AllergyIntolerance</v>
       </c>
       <c r="B30" t="str">
-        <v>code</v>
-      </c>
-      <c r="C30" t="str">
-        <v>coding</v>
+        <v>category</v>
       </c>
       <c r="E30" t="str">
         <v>array</v>
@@ -1275,16 +1248,16 @@
         <v>phenotypicFeatures</v>
       </c>
       <c r="I30" t="str">
-        <v>modifiers</v>
+        <v>featureType</v>
       </c>
       <c r="K30" t="str">
-        <v>array</v>
+        <v>object</v>
       </c>
       <c r="L30" t="str">
-        <v>TRANSFORM-id,label|Coding-system,code-unitcode,display</v>
+        <v>TRANSFORM-id,label|Default Value-type-code,value</v>
       </c>
       <c r="M30" t="str">
-        <v>[{"system":"http://snomed.info/sct","code":"SNOMED"},{"system":"http://loinc.org","code":"LOINC"},{"system":"http://unitsofmeasure.org","code":"UCUM"},{"system":"http://terminology.hl7.org/CodeSystem/condition-category","code":"HL7"},{"system":"http://hl7.org/fhir/sid/icd-10","code":"ICD10"},{"system":"http://www.whocc.no/atc","code":"WHO"},{"system":"http://terminology.kemkes.go.id/CodeSystem/clinical-term","code":"KEMKES"},{"system":"http://sys-ids.kemkes.go.id/kfa","code":"KFA"},{"system":"http://hl7.org/fhir/sid/icd-9-cm","code":"ICD9CM"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-topography","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-morphology","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-t-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-n-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-m-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/examination","code":"KEMKES"}]</v>
+        <v>[{"type":"environment","code":"SNOMED:414285001","value":"Allergy to substance (disorder)"},{"type":"medication","code":"SNOMED:416098002","value":"Drug allergy (disorder)"},{"type":"food","code":"SNOMED:426232007","value":"Allergy to food (disorder)"},{"type":"biologic","code":"FHIR:biologic","value":"Biologic"}]</v>
       </c>
     </row>
     <row r="31">
@@ -1295,10 +1268,10 @@
         <v>code</v>
       </c>
       <c r="C31" t="str">
-        <v>text</v>
+        <v>coding</v>
       </c>
       <c r="E31" t="str">
-        <v>string</v>
+        <v>array</v>
       </c>
       <c r="F31" t="str">
         <v>COMBINED</v>
@@ -1310,47 +1283,56 @@
         <v>phenotypicFeatures</v>
       </c>
       <c r="I31" t="str">
-        <v>notes</v>
+        <v>modifiers</v>
       </c>
       <c r="K31" t="str">
-        <v>string</v>
+        <v>array</v>
+      </c>
+      <c r="L31" t="str">
+        <v>TRANSFORM-id,label|Coding-system,code-unitcode,display</v>
+      </c>
+      <c r="M31" t="str">
+        <v>[{"system":"http://snomed.info/sct","code":"SNOMED"},{"system":"http://loinc.org","code":"LOINC"},{"system":"http://unitsofmeasure.org","code":"UCUM"},{"system":"http://terminology.hl7.org/CodeSystem/condition-category","code":"HL7"},{"system":"http://hl7.org/fhir/sid/icd-10","code":"ICD10"},{"system":"http://www.whocc.no/atc","code":"WHO"},{"system":"http://terminology.kemkes.go.id/CodeSystem/clinical-term","code":"KEMKES"},{"system":"http://sys-ids.kemkes.go.id/kfa","code":"KFA"},{"system":"http://hl7.org/fhir/sid/icd-9-cm","code":"ICD9CM"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-topography","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-morphology","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-t-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-n-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-m-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/examination","code":"KEMKES"}]</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>Medication</v>
+        <v>AllergyIntolerance</v>
+      </c>
+      <c r="B32" t="str">
+        <v>code</v>
+      </c>
+      <c r="C32" t="str">
+        <v>text</v>
       </c>
       <c r="E32" t="str">
-        <v>array</v>
+        <v>string</v>
       </c>
       <c r="F32" t="str">
-        <v>VALIDATE|status-string|completed||COMBINENEXT-1</v>
+        <v>COMBINED</v>
       </c>
       <c r="G32" t="str">
         <v>individuals</v>
       </c>
       <c r="H32" t="str">
-        <v>treatments</v>
+        <v>phenotypicFeatures</v>
+      </c>
+      <c r="I32" t="str">
+        <v>notes</v>
       </c>
       <c r="K32" t="str">
-        <v>array</v>
+        <v>string</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
         <v>Medication</v>
       </c>
-      <c r="B33" t="str">
-        <v>code</v>
-      </c>
-      <c r="C33" t="str">
-        <v>coding</v>
-      </c>
       <c r="E33" t="str">
         <v>array</v>
       </c>
       <c r="F33" t="str">
-        <v>COMBINED</v>
+        <v>VALIDATE|status-string|completed||COMBINENEXT-1</v>
       </c>
       <c r="G33" t="str">
         <v>individuals</v>
@@ -1358,28 +1340,25 @@
       <c r="H33" t="str">
         <v>treatments</v>
       </c>
-      <c r="I33" t="str">
-        <v>treatmentCode</v>
-      </c>
       <c r="K33" t="str">
-        <v>object</v>
-      </c>
-      <c r="L33" t="str">
-        <v>TRANSFORM-id,label|Coding-system,code-unitcode,display</v>
-      </c>
-      <c r="M33" t="str">
-        <v>[{"system":"http://snomed.info/sct","code":"SNOMED"},{"system":"http://loinc.org","code":"LOINC"},{"system":"http://unitsofmeasure.org","code":"UCUM"},{"system":"http://terminology.hl7.org/CodeSystem/condition-category","code":"HL7"},{"system":"http://hl7.org/fhir/sid/icd-10","code":"ICD10"},{"system":"http://www.whocc.no/atc","code":"WHO"},{"system":"http://terminology.kemkes.go.id/CodeSystem/clinical-term","code":"KEMKES"},{"system":"http://sys-ids.kemkes.go.id/kfa","code":"KFA"},{"system":"http://hl7.org/fhir/sid/icd-9-cm","code":"ICD9CM"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-topography","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-morphology","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-t-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-n-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-m-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/examination","code":"KEMKES"}]</v>
+        <v>array</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>MedicationDispense</v>
+        <v>Medication</v>
+      </c>
+      <c r="B34" t="str">
+        <v>code</v>
+      </c>
+      <c r="C34" t="str">
+        <v>coding</v>
       </c>
       <c r="E34" t="str">
         <v>array</v>
       </c>
       <c r="F34" t="str">
-        <v>VALIDATE|status-string|completed||COMBINENEXT-4</v>
+        <v>COMBINED</v>
       </c>
       <c r="G34" t="str">
         <v>individuals</v>
@@ -1387,25 +1366,28 @@
       <c r="H34" t="str">
         <v>treatments</v>
       </c>
+      <c r="I34" t="str">
+        <v>treatmentCode</v>
+      </c>
       <c r="K34" t="str">
-        <v>array</v>
+        <v>object</v>
+      </c>
+      <c r="L34" t="str">
+        <v>TRANSFORM-id,label|Coding-system,code-unitcode,display</v>
+      </c>
+      <c r="M34" t="str">
+        <v>[{"system":"http://snomed.info/sct","code":"SNOMED"},{"system":"http://loinc.org","code":"LOINC"},{"system":"http://unitsofmeasure.org","code":"UCUM"},{"system":"http://terminology.hl7.org/CodeSystem/condition-category","code":"HL7"},{"system":"http://hl7.org/fhir/sid/icd-10","code":"ICD10"},{"system":"http://www.whocc.no/atc","code":"WHO"},{"system":"http://terminology.kemkes.go.id/CodeSystem/clinical-term","code":"KEMKES"},{"system":"http://sys-ids.kemkes.go.id/kfa","code":"KFA"},{"system":"http://hl7.org/fhir/sid/icd-9-cm","code":"ICD9CM"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-topography","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-morphology","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-t-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-n-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-m-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/examination","code":"KEMKES"}]</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
         <v>MedicationDispense</v>
       </c>
-      <c r="B35" t="str">
-        <v>subject</v>
-      </c>
-      <c r="C35" t="str">
-        <v>reference</v>
-      </c>
       <c r="E35" t="str">
-        <v>string</v>
+        <v>array</v>
       </c>
       <c r="F35" t="str">
-        <v>COMBINED</v>
+        <v>VALIDATE|status-string|completed||COMBINENEXT-4</v>
       </c>
       <c r="G35" t="str">
         <v>individuals</v>
@@ -1413,14 +1395,8 @@
       <c r="H35" t="str">
         <v>treatments</v>
       </c>
-      <c r="I35" t="str">
-        <v>id</v>
-      </c>
       <c r="K35" t="str">
-        <v>string</v>
-      </c>
-      <c r="L35" t="str">
-        <v>TRANSFORM-id|SPLIT(/,-1)</v>
+        <v>array</v>
       </c>
     </row>
     <row r="36">
@@ -1428,13 +1404,13 @@
         <v>MedicationDispense</v>
       </c>
       <c r="B36" t="str">
-        <v>medicationCodeableConcept</v>
+        <v>subject</v>
       </c>
       <c r="C36" t="str">
-        <v>coding</v>
+        <v>reference</v>
       </c>
       <c r="E36" t="str">
-        <v>array</v>
+        <v>string</v>
       </c>
       <c r="F36" t="str">
         <v>COMBINED</v>
@@ -1446,16 +1422,13 @@
         <v>treatments</v>
       </c>
       <c r="I36" t="str">
-        <v>treatmentCode</v>
+        <v>id</v>
       </c>
       <c r="K36" t="str">
-        <v>object</v>
+        <v>string</v>
       </c>
       <c r="L36" t="str">
-        <v>TRANSFORM-id,label|Coding-system,code-unitcode,display</v>
-      </c>
-      <c r="M36" t="str">
-        <v>[{"system":"http://snomed.info/sct","code":"SNOMED"},{"system":"http://loinc.org","code":"LOINC"},{"system":"http://unitsofmeasure.org","code":"UCUM"},{"system":"http://terminology.hl7.org/CodeSystem/condition-category","code":"HL7"},{"system":"http://hl7.org/fhir/sid/icd-10","code":"ICD10"},{"system":"http://www.whocc.no/atc","code":"WHO"},{"system":"http://terminology.kemkes.go.id/CodeSystem/clinical-term","code":"KEMKES"},{"system":"http://sys-ids.kemkes.go.id/kfa","code":"KFA"},{"system":"http://hl7.org/fhir/sid/icd-9-cm","code":"ICD9CM"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-topography","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-morphology","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-t-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-n-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-m-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/examination","code":"KEMKES"}]</v>
+        <v>TRANSFORM-id|SPLIT(/,-1)</v>
       </c>
     </row>
     <row r="37">
@@ -1463,12 +1436,9 @@
         <v>MedicationDispense</v>
       </c>
       <c r="B37" t="str">
-        <v>dosageInstruction</v>
+        <v>medicationCodeableConcept</v>
       </c>
       <c r="C37" t="str">
-        <v>route</v>
-      </c>
-      <c r="D37" t="str">
         <v>coding</v>
       </c>
       <c r="E37" t="str">
@@ -1484,7 +1454,7 @@
         <v>treatments</v>
       </c>
       <c r="I37" t="str">
-        <v>routeOfAdministration</v>
+        <v>treatmentCode</v>
       </c>
       <c r="K37" t="str">
         <v>object</v>
@@ -1504,10 +1474,10 @@
         <v>dosageInstruction</v>
       </c>
       <c r="C38" t="str">
-        <v>doseAndRate</v>
+        <v>route</v>
       </c>
       <c r="D38" t="str">
-        <v>doseQuantity</v>
+        <v>coding</v>
       </c>
       <c r="E38" t="str">
         <v>array</v>
@@ -1522,16 +1492,13 @@
         <v>treatments</v>
       </c>
       <c r="I38" t="str">
-        <v>doseIntervals</v>
-      </c>
-      <c r="J38" t="str">
-        <v>quantity</v>
+        <v>routeOfAdministration</v>
       </c>
       <c r="K38" t="str">
         <v>object</v>
       </c>
       <c r="L38" t="str">
-        <v>TRANSFORM-unit[id:label],value|Value-system,code-[unitcode:code],value</v>
+        <v>TRANSFORM-id,label|Coding-system,code-unitcode,display</v>
       </c>
       <c r="M38" t="str">
         <v>[{"system":"http://snomed.info/sct","code":"SNOMED"},{"system":"http://loinc.org","code":"LOINC"},{"system":"http://unitsofmeasure.org","code":"UCUM"},{"system":"http://terminology.hl7.org/CodeSystem/condition-category","code":"HL7"},{"system":"http://hl7.org/fhir/sid/icd-10","code":"ICD10"},{"system":"http://www.whocc.no/atc","code":"WHO"},{"system":"http://terminology.kemkes.go.id/CodeSystem/clinical-term","code":"KEMKES"},{"system":"http://sys-ids.kemkes.go.id/kfa","code":"KFA"},{"system":"http://hl7.org/fhir/sid/icd-9-cm","code":"ICD9CM"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-topography","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-morphology","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-t-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-n-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-m-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/examination","code":"KEMKES"}]</v>
@@ -1539,39 +1506,54 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>FamilyMemberHistory</v>
+        <v>MedicationDispense</v>
+      </c>
+      <c r="B39" t="str">
+        <v>dosageInstruction</v>
+      </c>
+      <c r="C39" t="str">
+        <v>doseAndRate</v>
+      </c>
+      <c r="D39" t="str">
+        <v>doseQuantity</v>
       </c>
       <c r="E39" t="str">
         <v>array</v>
       </c>
       <c r="F39" t="str">
-        <v>VALIDATE|status-string|completed||COMBINENEXT-2|GET-2-code-coding</v>
+        <v>COMBINED</v>
       </c>
       <c r="G39" t="str">
         <v>individuals</v>
       </c>
       <c r="H39" t="str">
-        <v>diseases</v>
+        <v>treatments</v>
+      </c>
+      <c r="I39" t="str">
+        <v>doseIntervals</v>
+      </c>
+      <c r="J39" t="str">
+        <v>quantity</v>
       </c>
       <c r="K39" t="str">
-        <v>array</v>
+        <v>object</v>
+      </c>
+      <c r="L39" t="str">
+        <v>TRANSFORM-unit[id:label],value|Value-system,code-[unitcode:code],value</v>
+      </c>
+      <c r="M39" t="str">
+        <v>[{"system":"http://snomed.info/sct","code":"SNOMED"},{"system":"http://loinc.org","code":"LOINC"},{"system":"http://unitsofmeasure.org","code":"UCUM"},{"system":"http://terminology.hl7.org/CodeSystem/condition-category","code":"HL7"},{"system":"http://hl7.org/fhir/sid/icd-10","code":"ICD10"},{"system":"http://www.whocc.no/atc","code":"WHO"},{"system":"http://terminology.kemkes.go.id/CodeSystem/clinical-term","code":"KEMKES"},{"system":"http://sys-ids.kemkes.go.id/kfa","code":"KFA"},{"system":"http://hl7.org/fhir/sid/icd-9-cm","code":"ICD9CM"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-topography","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-morphology","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-t-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-n-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-m-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/examination","code":"KEMKES"}]</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
         <v>FamilyMemberHistory</v>
       </c>
-      <c r="B40" t="str">
-        <v>patient</v>
-      </c>
-      <c r="C40" t="str">
-        <v>reference</v>
-      </c>
       <c r="E40" t="str">
-        <v>string</v>
+        <v>array</v>
       </c>
       <c r="F40" t="str">
-        <v>COMBINED</v>
+        <v>VALIDATE|status-string|completed||COMBINENEXT-2|GET-2-code-coding</v>
       </c>
       <c r="G40" t="str">
         <v>individuals</v>
@@ -1579,14 +1561,8 @@
       <c r="H40" t="str">
         <v>diseases</v>
       </c>
-      <c r="I40" t="str">
-        <v>id</v>
-      </c>
       <c r="K40" t="str">
-        <v>string</v>
-      </c>
-      <c r="L40" t="str">
-        <v>TRANSFORM-id|SPLIT(/,-1)</v>
+        <v>array</v>
       </c>
     </row>
     <row r="41">
@@ -1594,10 +1570,13 @@
         <v>FamilyMemberHistory</v>
       </c>
       <c r="B41" t="str">
-        <v>condition</v>
+        <v>patient</v>
+      </c>
+      <c r="C41" t="str">
+        <v>reference</v>
       </c>
       <c r="E41" t="str">
-        <v>array</v>
+        <v>string</v>
       </c>
       <c r="F41" t="str">
         <v>COMBINED</v>
@@ -1609,21 +1588,50 @@
         <v>diseases</v>
       </c>
       <c r="I41" t="str">
+        <v>id</v>
+      </c>
+      <c r="K41" t="str">
+        <v>string</v>
+      </c>
+      <c r="L41" t="str">
+        <v>TRANSFORM-id|SPLIT(/,-1)</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>FamilyMemberHistory</v>
+      </c>
+      <c r="B42" t="str">
+        <v>condition</v>
+      </c>
+      <c r="E42" t="str">
+        <v>array</v>
+      </c>
+      <c r="F42" t="str">
+        <v>COMBINED</v>
+      </c>
+      <c r="G42" t="str">
+        <v>individuals</v>
+      </c>
+      <c r="H42" t="str">
+        <v>diseases</v>
+      </c>
+      <c r="I42" t="str">
         <v>diseaseCode</v>
       </c>
-      <c r="K41" t="str">
+      <c r="K42" t="str">
         <v>object</v>
       </c>
-      <c r="L41" t="str">
+      <c r="L42" t="str">
         <v>TRANSFORM-id,label|Coding-system,code-unitcode,display</v>
       </c>
-      <c r="M41" t="str">
+      <c r="M42" t="str">
         <v>[{"system":"http://snomed.info/sct","code":"SNOMED"},{"system":"http://loinc.org","code":"LOINC"},{"system":"http://unitsofmeasure.org","code":"UCUM"},{"system":"http://terminology.hl7.org/CodeSystem/condition-category","code":"HL7"},{"system":"http://hl7.org/fhir/sid/icd-10","code":"ICD10"},{"system":"http://www.whocc.no/atc","code":"WHO"},{"system":"http://terminology.kemkes.go.id/CodeSystem/clinical-term","code":"KEMKES"},{"system":"http://sys-ids.kemkes.go.id/kfa","code":"KFA"},{"system":"http://hl7.org/fhir/sid/icd-9-cm","code":"ICD9CM"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-topography","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-morphology","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-t-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-n-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-m-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/examination","code":"KEMKES"}]</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M41"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M42"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
remove id from dieases
</commit_message>
<xml_diff>
--- a/Mapper.xlsx
+++ b/Mapper.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SafrialWiguna\source\repos\swrepo14461\ETL-FHIR-Beacon\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2301BDA2-55B9-4C33-9283-18C78DB26957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Mapper" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Old_Mapper" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Mapper" sheetId="1" r:id="rId1"/>
+    <sheet name="Old_Mapper" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Mapper!$A$1:$M$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Mapper!$A$1:$M$34</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -24,491 +29,490 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="158">
-  <si>
-    <t xml:space="preserve">Where to Find</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What to Find First</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What to Find Second</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What to Find Third</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type of Find Used</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What to Do</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Where to Use</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What to Use First</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What to Use Second</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What to Use Third</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type of Use Used</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What Must Be Done</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AllergyIntolerance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">array</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDATE|clinicalStatus-object,coding-array,code-string|active||COMBINENEXT-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">individual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phenotypicFeatures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">patient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">string</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMBINED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">featureType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">object</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRANSFORM-id|Default Value-type-code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[{"type":"environment","code":"SNOMED:414285001","value":"Allergy to substance (disorder)"},{"type":"medication","code":"SNOMED:416098002","value":"Drug allergy (disorder)"},{"type":"food","code":"SNOMED:426232007","value":"Allergy to food (disorder)"},{"type":"biologic","code":"FHIR:biologic","value":"Biologic"}]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">coding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">modifiers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRANSFORM-id,label|Coding-system,code-unitcode,display</t>
-  </si>
-  <si>
-    <t xml:space="preserve">text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Condition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDATE|clinicalStatus-object,coding-array,code-string|active||COMBINENEXT-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diseases</t>
-  </si>
-  <si>
-    <t xml:space="preserve">subject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diseaseCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FamilyMemberHistory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDATE|status-string|completed||COMBINENEXT-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">familyHistory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">boolean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRANSFORMTOBOOLEAN|completed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">condition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMBINED|GET-code-coding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Immunization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">measurements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vaccineCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">procedure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medication</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMBINENEXT-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">treatments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">treatmentCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MedicationDispense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDATE|status-string|completed||COMBINENEXT-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dosageInstruction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMBINED|GET-route-coding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">routeOfAdministration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMBINED|GET-doseAndRate-doseQuantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">doseIntervals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">quantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRANSFORM-unit[id:label],value|Value-system,code-[unitcode:code],value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMBINED|GET-timing-repeat-boundsPeriod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">interval</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRANSFORM-start,end|DATETIME-start,end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">medicationCodeableConcept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NutritionOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDATE|status-string|activeORcompleted||COMBINENEXT-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oralDiet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMBINED|GET-coding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phenotypicFeature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nutrient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMBINED|GET-modifier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMBINED|GET-amount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cumulativeDose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enteralFormula</t>
-  </si>
-  <si>
-    <t xml:space="preserve">baseFormulaType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">treatmentsCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">administration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMBINED|GET-quantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">routeofAdministration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Observation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDATE|status-string|completedORfinal||VALIDATE|category-array,coding-array,code-string|vital-signsORlaboratory||COMBINENEXT-9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assayCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">valueQuantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">measurementValue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[{"system":"http://snomed.info/sct","code":"SNOMED"},{"system":"http://loinc.org","code":"LOINC"},{"system":"http://unitsofmeasure.org","code":"UCUM"},{"system":"http://terminology.hl7.org/CodeSystem/condition-category","code":"HL7"},{"system":"http://hl7.org/fhir/sid/icd-10","code":"ICD10"},{"system":"http://www.whocc.no/atc","code":"WHO"},{"system":"http://terminology.kemkes.go.id/CodeSystem/clinical-term","code":"KEMKES"},{"system":"http://sys-ids.kemkes.go.id/kfa","code":"KFA"},{"system":"http://hl7.org/fhir/sid/icd-9-cm","code":"ICD9CM"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-topography","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-morphology","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-t-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-n-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-m-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/examination","code":"KEMKES"}]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">issued</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">component</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRANSFORM-typedQuantities[quantityType[id:label]]|Value-system,code-[unitcode:code],value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMBINED|GET-valueQuantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRANSFORM-typedQuantities[quantityType[unit[id:label]:value]]|Value-system,code-[unitcode:code],value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">interpretation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMBINED|GET-coding-display</t>
-  </si>
-  <si>
-    <t xml:space="preserve">referenceRange</t>
-  </si>
-  <si>
-    <t xml:space="preserve">low</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRANSFORM-referenceRange[low:unit[id:label]]|Value-system,code-[unitcode:code],value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">high</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRANSFORM-referenceRange[id:label],value|Value-system,code-[unitcode:code],value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDATE|status-string|completedORfinal||VALIDATE|category-array,coding-array,code-string|examORimaging||VALIDATE-HAD|component-array||COMBINENEXT-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDATE-NOT|component-array,code-object,coding-array,system-string|http://snomed.info/sct||COMBINED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDATE-NOT|component-array,code-object,coding-array,system-string|http://snomed.info/sct||COMBINED|GET-code-coding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDATE-NOT|component-array,code-object,coding-array,system-string|http://snomed.info/sct||COMBINED|GET-valueCodeableConcept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">severity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDATE-NOT|component-array,code-object,coding-array,system-string|http://snomed.info/sct||COMBINED|GET-valueBoolean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">excluded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDATE|component-array,code-object,coding-array,system-string|http://snomed.info/sct||COMBINED|GET-valueCodeableConcept</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diseasesCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDATE|component-array,code-object,coding-array,system-string|http://snomed.info/sct||COMBINED|GET-valueString</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDATE|category-array,coding-array,code-string|procedureORimaging||COMBINENEXT-5||VALIDATE|status-string|completedORfinal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">interventionsOrProcedures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">procedureCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">effectiveDateTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dateOfProcedure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">valueString</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRANSFORM-id,label|Default Value-value-code,value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[{"code":"NCIT:C17998","value":"unknown","description":"Not assessed or not available."},{"code":"NCIT:C16576","value":"female","description":"Female."},{"code":"NCIT:C20197","value":"male","description":"Male."}]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">birthDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">datetime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRANSFORMDATETOAGE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">identifier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPLIT-/-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Procedure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specimen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDATE|status-string|available||COMBINENEXT-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biosample</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biosampleStatus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">method</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sampleOriginType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ServiceRequest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDATE|status-string|activeORCompleted||VALIDATE|category-array,code-string|108252007||COMBINENEXT-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDATE|status-string|final||COMBINENEXT-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">valueBoolean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">valueInteger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDATE|status-string|final||VALIDATE-NOT|component-array,code-object,coding-array,system-string|http://snomed.info/sct||COMBINENEXT-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDATE|valueBoolean|true</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMBINED|GET-valueCodeableConcept-coding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMBINED|GET-valueString</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDATE|status-string|final||VALIDATE|component-array,code-object,coding-array,system-string|http://snomed.info/sct||COMBINENEXT-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDATE|status-string|completed||COMBINENEXT-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">performedDateTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRANSFORM-id,label|Default Value-type-code,value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MedicationRequest/MedicationDispense</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDATE|status-string|activeORcompleted||COMBINENEXT-2-MedicationDispense||COMBINENEXT-4-MedicationRequest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">medicationReference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMBINED|GETREF-code-coding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MedicationRequest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALIDATE|status-string|activeORcompleted||COMBINENEXT-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nutrition</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="159">
+  <si>
+    <t>Where to Find</t>
+  </si>
+  <si>
+    <t>What to Find First</t>
+  </si>
+  <si>
+    <t>What to Find Second</t>
+  </si>
+  <si>
+    <t>What to Find Third</t>
+  </si>
+  <si>
+    <t>Type of Find Used</t>
+  </si>
+  <si>
+    <t>What to Do</t>
+  </si>
+  <si>
+    <t>Where to Use</t>
+  </si>
+  <si>
+    <t>What to Use First</t>
+  </si>
+  <si>
+    <t>What to Use Second</t>
+  </si>
+  <si>
+    <t>What to Use Third</t>
+  </si>
+  <si>
+    <t>Type of Use Used</t>
+  </si>
+  <si>
+    <t>What Must Be Done</t>
+  </si>
+  <si>
+    <t>Default Value</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance</t>
+  </si>
+  <si>
+    <t>array</t>
+  </si>
+  <si>
+    <t>VALIDATE|clinicalStatus-object,coding-array,code-string|active||COMBINENEXT-4</t>
+  </si>
+  <si>
+    <t>individual</t>
+  </si>
+  <si>
+    <t>phenotypicFeatures</t>
+  </si>
+  <si>
+    <t>patient</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>COMBINED</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>featureType</t>
+  </si>
+  <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>TRANSFORM-id|Default Value-type-code</t>
+  </si>
+  <si>
+    <t>[{"type":"environment","code":"SNOMED:414285001","value":"Allergy to substance (disorder)"},{"type":"medication","code":"SNOMED:416098002","value":"Drug allergy (disorder)"},{"type":"food","code":"SNOMED:426232007","value":"Allergy to food (disorder)"},{"type":"biologic","code":"FHIR:biologic","value":"Biologic"}]</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>coding</t>
+  </si>
+  <si>
+    <t>modifiers</t>
+  </si>
+  <si>
+    <t>TRANSFORM-id,label|Coding-system,code-unitcode,display</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>VALIDATE|clinicalStatus-object,coding-array,code-string|active||COMBINENEXT-3</t>
+  </si>
+  <si>
+    <t>diseases</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>diseaseCode</t>
+  </si>
+  <si>
+    <t>FamilyMemberHistory</t>
+  </si>
+  <si>
+    <t>VALIDATE|status-string|completed||COMBINENEXT-2</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>familyHistory</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>TRANSFORMTOBOOLEAN|completed</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>COMBINED|GET-code-coding</t>
+  </si>
+  <si>
+    <t>Immunization</t>
+  </si>
+  <si>
+    <t>measurements</t>
+  </si>
+  <si>
+    <t>vaccineCode</t>
+  </si>
+  <si>
+    <t>procedure</t>
+  </si>
+  <si>
+    <t>Medication</t>
+  </si>
+  <si>
+    <t>COMBINENEXT-1</t>
+  </si>
+  <si>
+    <t>treatments</t>
+  </si>
+  <si>
+    <t>treatmentCode</t>
+  </si>
+  <si>
+    <t>MedicationDispense</t>
+  </si>
+  <si>
+    <t>VALIDATE|status-string|completed||COMBINENEXT-5</t>
+  </si>
+  <si>
+    <t>dosageInstruction</t>
+  </si>
+  <si>
+    <t>COMBINED|GET-route-coding</t>
+  </si>
+  <si>
+    <t>routeOfAdministration</t>
+  </si>
+  <si>
+    <t>COMBINED|GET-doseAndRate-doseQuantity</t>
+  </si>
+  <si>
+    <t>doseIntervals</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>TRANSFORM-unit[id:label],value|Value-system,code-[unitcode:code],value</t>
+  </si>
+  <si>
+    <t>COMBINED|GET-timing-repeat-boundsPeriod</t>
+  </si>
+  <si>
+    <t>interval</t>
+  </si>
+  <si>
+    <t>TRANSFORM-start,end|DATETIME-start,end</t>
+  </si>
+  <si>
+    <t>medicationCodeableConcept</t>
+  </si>
+  <si>
+    <t>NutritionOrder</t>
+  </si>
+  <si>
+    <t>VALIDATE|status-string|activeORcompleted||COMBINENEXT-7</t>
+  </si>
+  <si>
+    <t>oralDiet</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>COMBINED|GET-coding</t>
+  </si>
+  <si>
+    <t>phenotypicFeature</t>
+  </si>
+  <si>
+    <t>nutrient</t>
+  </si>
+  <si>
+    <t>COMBINED|GET-modifier</t>
+  </si>
+  <si>
+    <t>COMBINED|GET-amount</t>
+  </si>
+  <si>
+    <t>cumulativeDose</t>
+  </si>
+  <si>
+    <t>enteralFormula</t>
+  </si>
+  <si>
+    <t>baseFormulaType</t>
+  </si>
+  <si>
+    <t>treatmentsCode</t>
+  </si>
+  <si>
+    <t>administration</t>
+  </si>
+  <si>
+    <t>COMBINED|GET-quantity</t>
+  </si>
+  <si>
+    <t>routeofAdministration</t>
+  </si>
+  <si>
+    <t>Observation</t>
+  </si>
+  <si>
+    <t>VALIDATE|status-string|completedORfinal||VALIDATE|category-array,coding-array,code-string|vital-signsORlaboratory||COMBINENEXT-9</t>
+  </si>
+  <si>
+    <t>assayCode</t>
+  </si>
+  <si>
+    <t>valueQuantity</t>
+  </si>
+  <si>
+    <t>measurementValue</t>
+  </si>
+  <si>
+    <t>[{"system":"http://snomed.info/sct","code":"SNOMED"},{"system":"http://loinc.org","code":"LOINC"},{"system":"http://unitsofmeasure.org","code":"UCUM"},{"system":"http://terminology.hl7.org/CodeSystem/condition-category","code":"HL7"},{"system":"http://hl7.org/fhir/sid/icd-10","code":"ICD10"},{"system":"http://www.whocc.no/atc","code":"WHO"},{"system":"http://terminology.kemkes.go.id/CodeSystem/clinical-term","code":"KEMKES"},{"system":"http://sys-ids.kemkes.go.id/kfa","code":"KFA"},{"system":"http://hl7.org/fhir/sid/icd-9-cm","code":"ICD9CM"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-topography","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/icd-o-morphology","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-t-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-n-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/cancer-m-category","code":"KEMKES"},{"system":"http://terminology.kemkes.go.id/CodeSystem/examination","code":"KEMKES"}]</t>
+  </si>
+  <si>
+    <t>issued</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>TRANSFORM-typedQuantities[quantityType[id:label]]|Value-system,code-[unitcode:code],value</t>
+  </si>
+  <si>
+    <t>COMBINED|GET-valueQuantity</t>
+  </si>
+  <si>
+    <t>TRANSFORM-typedQuantities[quantityType[unit[id:label]:value]]|Value-system,code-[unitcode:code],value</t>
+  </si>
+  <si>
+    <t>interpretation</t>
+  </si>
+  <si>
+    <t>COMBINED|GET-coding-display</t>
+  </si>
+  <si>
+    <t>referenceRange</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>TRANSFORM-referenceRange[low:unit[id:label]]|Value-system,code-[unitcode:code],value</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>TRANSFORM-referenceRange[id:label],value|Value-system,code-[unitcode:code],value</t>
+  </si>
+  <si>
+    <t>VALIDATE|status-string|completedORfinal||VALIDATE|category-array,coding-array,code-string|examORimaging||VALIDATE-HAD|component-array||COMBINENEXT-7</t>
+  </si>
+  <si>
+    <t>VALIDATE-NOT|component-array,code-object,coding-array,system-string|http://snomed.info/sct||COMBINED</t>
+  </si>
+  <si>
+    <t>VALIDATE-NOT|component-array,code-object,coding-array,system-string|http://snomed.info/sct||COMBINED|GET-code-coding</t>
+  </si>
+  <si>
+    <t>VALIDATE-NOT|component-array,code-object,coding-array,system-string|http://snomed.info/sct||COMBINED|GET-valueCodeableConcept</t>
+  </si>
+  <si>
+    <t>severity</t>
+  </si>
+  <si>
+    <t>VALIDATE-NOT|component-array,code-object,coding-array,system-string|http://snomed.info/sct||COMBINED|GET-valueBoolean</t>
+  </si>
+  <si>
+    <t>excluded</t>
+  </si>
+  <si>
+    <t>VALIDATE|component-array,code-object,coding-array,system-string|http://snomed.info/sct||COMBINED|GET-valueCodeableConcept</t>
+  </si>
+  <si>
+    <t>diseasesCode</t>
+  </si>
+  <si>
+    <t>VALIDATE|component-array,code-object,coding-array,system-string|http://snomed.info/sct||COMBINED|GET-valueString</t>
+  </si>
+  <si>
+    <t>VALIDATE|category-array,coding-array,code-string|procedureORimaging||COMBINENEXT-5||VALIDATE|status-string|completedORfinal</t>
+  </si>
+  <si>
+    <t>interventionsOrProcedures</t>
+  </si>
+  <si>
+    <t>procedureCode</t>
+  </si>
+  <si>
+    <t>effectiveDateTime</t>
+  </si>
+  <si>
+    <t>dateOfProcedure</t>
+  </si>
+  <si>
+    <t>valueString</t>
+  </si>
+  <si>
+    <t>Patient</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>TRANSFORM-id,label|Default Value-value-code,value</t>
+  </si>
+  <si>
+    <t>[{"code":"NCIT:C17998","value":"unknown","description":"Not assessed or not available."},{"code":"NCIT:C16576","value":"female","description":"Female."},{"code":"NCIT:C20197","value":"male","description":"Male."}]</t>
+  </si>
+  <si>
+    <t>birthDate</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>TRANSFORMDATETOAGE</t>
+  </si>
+  <si>
+    <t>identifier</t>
+  </si>
+  <si>
+    <t>SPLIT-/-1</t>
+  </si>
+  <si>
+    <t>Procedure</t>
+  </si>
+  <si>
+    <t>Specimen</t>
+  </si>
+  <si>
+    <t>VALIDATE|status-string|available||COMBINENEXT-3</t>
+  </si>
+  <si>
+    <t>biosample</t>
+  </si>
+  <si>
+    <t>biosampleStatus</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>sampleOriginType</t>
+  </si>
+  <si>
+    <t>ServiceRequest</t>
+  </si>
+  <si>
+    <t>VALIDATE|status-string|activeORCompleted||VALIDATE|category-array,code-string|108252007||COMBINENEXT-1</t>
+  </si>
+  <si>
+    <t>VALIDATE|status-string|final||COMBINENEXT-6</t>
+  </si>
+  <si>
+    <t>valueBoolean</t>
+  </si>
+  <si>
+    <t>valueInteger</t>
+  </si>
+  <si>
+    <t>VALIDATE|status-string|final||VALIDATE-NOT|component-array,code-object,coding-array,system-string|http://snomed.info/sct||COMBINENEXT-5</t>
+  </si>
+  <si>
+    <t>VALIDATE|valueBoolean|true</t>
+  </si>
+  <si>
+    <t>COMBINED|GET-valueCodeableConcept-coding</t>
+  </si>
+  <si>
+    <t>COMBINED|GET-valueString</t>
+  </si>
+  <si>
+    <t>VALIDATE|status-string|final||VALIDATE|component-array,code-object,coding-array,system-string|http://snomed.info/sct||COMBINENEXT-1</t>
+  </si>
+  <si>
+    <t>VALIDATE|status-string|completed||COMBINENEXT-3</t>
+  </si>
+  <si>
+    <t>performedDateTime</t>
+  </si>
+  <si>
+    <t>TRANSFORM-id,label|Default Value-type-code,value</t>
+  </si>
+  <si>
+    <t>MedicationRequest/MedicationDispense</t>
+  </si>
+  <si>
+    <t>VALIDATE|status-string|activeORcompleted||COMBINENEXT-2-MedicationDispense||COMBINENEXT-4-MedicationRequest</t>
+  </si>
+  <si>
+    <t>medicationReference</t>
+  </si>
+  <si>
+    <t>COMBINED|GETREF-code-coding</t>
+  </si>
+  <si>
+    <t>MedicationRequest</t>
+  </si>
+  <si>
+    <t>VALIDATE|status-string|activeORcompleted||COMBINENEXT-2</t>
+  </si>
+  <si>
+    <t>nutrition</t>
+  </si>
+  <si>
+    <t>VALIDATE|clinicalStatus-object,coding-array,code-string|active||COMBINENEXT-2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -517,22 +521,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <u val="single"/>
+      <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Aptos Narrow"/>
@@ -547,7 +536,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -558,7 +547,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -585,13 +573,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.15"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -599,111 +587,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="3">
+    <cellStyle name="Hipertaut 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Hipertaut 2" xfId="20"/>
-    <cellStyle name="Normal 2" xfId="21"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9D9D9"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -762,64 +675,76 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0e2841"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e8e8e8"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="e97132"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196b24"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0f9ed5"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="a02b93"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4ea72e"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607d"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -851,7 +776,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -875,7 +800,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -935,42 +860,41 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:M69"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M53" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M59" activeCellId="0" sqref="M59"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="17.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="120.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="193.86"/>
+    <col min="1" max="1" width="37.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="17.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="120.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="69" style="1" customWidth="1"/>
+    <col min="13" max="13" width="193.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1011,7 +935,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1031,7 +955,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -1060,7 +984,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1092,7 +1016,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1124,7 +1048,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -1153,7 +1077,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
@@ -1161,7 +1085,7 @@
         <v>14</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>35</v>
+        <v>158</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>16</v>
@@ -1173,18 +1097,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>21</v>
@@ -1196,13 +1120,16 @@
         <v>36</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
@@ -1210,10 +1137,10 @@
         <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>21</v>
@@ -1225,30 +1152,21 @@
         <v>36</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>16</v>
@@ -1256,22 +1174,22 @@
       <c r="H10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="K10" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="B11" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="E11" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>16</v>
@@ -1279,22 +1197,28 @@
       <c r="H11" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="I11" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="K11" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>16</v>
@@ -1303,53 +1227,50 @@
         <v>36</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>38</v>
+      <c r="H13" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="4" t="s">
         <v>47</v>
       </c>
+      <c r="B14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E14" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>16</v>
@@ -1357,22 +1278,25 @@
       <c r="H14" s="5" t="s">
         <v>48</v>
       </c>
+      <c r="I14" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="K14" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>21</v>
@@ -1384,53 +1308,50 @@
         <v>48</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H16" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>50</v>
+      <c r="H16" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="4" t="s">
         <v>51</v>
       </c>
+      <c r="B17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="E17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>16</v>
@@ -1438,25 +1359,25 @@
       <c r="H17" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="I17" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="K17" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>16</v>
@@ -1464,25 +1385,25 @@
       <c r="H18" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="K18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E19" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>16</v>
@@ -1490,25 +1411,25 @@
       <c r="H19" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="I19" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="K19" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>16</v>
@@ -1517,13 +1438,16 @@
         <v>53</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="1" t="s">
         <v>55</v>
       </c>
@@ -1534,7 +1458,7 @@
         <v>14</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>16</v>
@@ -1543,16 +1467,19 @@
         <v>53</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
@@ -1563,7 +1490,7 @@
         <v>14</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>16</v>
@@ -1575,27 +1502,30 @@
         <v>61</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>57</v>
+        <v>67</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>16</v>
@@ -1604,33 +1534,24 @@
         <v>53</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>25</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>16</v>
@@ -1638,25 +1559,25 @@
       <c r="H24" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I24" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="K24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="B25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E25" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>16</v>
@@ -1664,40 +1585,46 @@
       <c r="H25" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="I25" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="K25" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="4" t="s">
         <v>68</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" s="4" t="s">
         <v>68</v>
       </c>
@@ -1705,13 +1632,13 @@
         <v>70</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>16</v>
@@ -1720,7 +1647,7 @@
         <v>73</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>25</v>
@@ -1729,7 +1656,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:12" s="1" customFormat="1">
       <c r="A28" s="4" t="s">
         <v>68</v>
       </c>
@@ -1743,39 +1670,42 @@
         <v>14</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>25</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" s="4" t="s">
         <v>68</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>16</v>
@@ -1784,16 +1714,16 @@
         <v>53</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>25</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="4" t="s">
         <v>68</v>
       </c>
@@ -1801,16 +1731,13 @@
         <v>78</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>16</v>
@@ -1819,16 +1746,16 @@
         <v>53</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>25</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" s="4" t="s">
         <v>68</v>
       </c>
@@ -1836,13 +1763,16 @@
         <v>78</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>82</v>
+        <v>21</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>16</v>
@@ -1851,59 +1781,50 @@
         <v>53</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>25</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>29</v>
+        <v>84</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>83</v>
+      <c r="H32" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" s="4" t="s">
         <v>84</v>
       </c>
+      <c r="B33" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E33" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>16</v>
@@ -1911,22 +1832,25 @@
       <c r="H33" s="5" t="s">
         <v>48</v>
       </c>
+      <c r="I33" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="K33" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>21</v>
@@ -1934,28 +1858,28 @@
       <c r="G34" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="H34" s="1" t="s">
         <v>48</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>22</v>
+        <v>86</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>21</v>
@@ -1967,24 +1891,27 @@
         <v>48</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>25</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>63</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>21</v>
@@ -1996,30 +1923,24 @@
         <v>48</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L36" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>16</v>
@@ -2028,13 +1949,16 @@
         <v>48</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38" s="1" t="s">
         <v>84</v>
       </c>
@@ -2045,7 +1969,7 @@
         <v>14</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>16</v>
@@ -2060,21 +1984,21 @@
         <v>25</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
       <c r="A39" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>16</v>
@@ -2083,27 +2007,27 @@
         <v>48</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L39" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
       <c r="A40" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>16</v>
@@ -2112,13 +2036,16 @@
         <v>48</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
       <c r="A41" s="1" t="s">
         <v>84</v>
       </c>
@@ -2126,7 +2053,7 @@
         <v>98</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>25</v>
@@ -2143,55 +2070,49 @@
       <c r="I41" s="1" t="s">
         <v>88</v>
       </c>
+      <c r="J41" s="6"/>
       <c r="K41" s="1" t="s">
         <v>25</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="E42" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>21</v>
+        <v>103</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="J42" s="6"/>
+        <v>17</v>
+      </c>
       <c r="K42" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
       <c r="A43" s="4" t="s">
         <v>84</v>
       </c>
+      <c r="B43" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E43" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>16</v>
@@ -2199,22 +2120,25 @@
       <c r="H43" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="I43" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="K43" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>104</v>
@@ -2226,27 +2150,27 @@
         <v>17</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
       <c r="A45" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>104</v>
+      <c r="F45" t="s">
+        <v>105</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>16</v>
@@ -2255,16 +2179,16 @@
         <v>17</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
       <c r="A46" s="1" t="s">
         <v>84</v>
       </c>
@@ -2274,8 +2198,8 @@
       <c r="E46" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F46" s="7" t="s">
-        <v>105</v>
+      <c r="F46" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>16</v>
@@ -2284,16 +2208,16 @@
         <v>17</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>30</v>
+        <v>107</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
       <c r="A47" s="1" t="s">
         <v>84</v>
       </c>
@@ -2304,7 +2228,7 @@
         <v>14</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>16</v>
@@ -2313,16 +2237,13 @@
         <v>17</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L47" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
       <c r="A48" s="1" t="s">
         <v>84</v>
       </c>
@@ -2333,33 +2254,37 @@
         <v>14</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
       <c r="A49" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>92</v>
       </c>
+      <c r="C49"/>
       <c r="E49" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>16</v>
@@ -2368,51 +2293,47 @@
         <v>36</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>111</v>
+        <v>33</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L49" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C50" s="0"/>
       <c r="E50" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>33</v>
+        <v>114</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
       <c r="A51" s="4" t="s">
         <v>84</v>
       </c>
+      <c r="B51" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="E51" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>113</v>
+        <v>21</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>16</v>
@@ -2420,22 +2341,25 @@
       <c r="H51" s="1" t="s">
         <v>114</v>
       </c>
+      <c r="I51" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="K51" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="4" t="s">
+      <c r="L51" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>29</v>
+        <v>116</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>21</v>
@@ -2447,21 +2371,18 @@
         <v>114</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L52" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
       <c r="A53" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>20</v>
@@ -2476,51 +2397,55 @@
         <v>114</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>117</v>
+        <v>33</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:13">
       <c r="A54" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>118</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="C54"/>
       <c r="E54" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>21</v>
+        <v>110</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>114</v>
+        <v>36</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>33</v>
+        <v>111</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
       <c r="A55" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C55" s="0"/>
+      <c r="C55"/>
       <c r="E55" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>16</v>
@@ -2529,48 +2454,38 @@
         <v>36</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>111</v>
+        <v>33</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L55" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
       <c r="A56" s="1" t="s">
-        <v>84</v>
+        <v>119</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C56" s="0"/>
+        <v>22</v>
+      </c>
       <c r="E56" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>112</v>
+        <v>20</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:13">
       <c r="A57" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>22</v>
+        <v>120</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>20</v>
@@ -2579,96 +2494,102 @@
         <v>16</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>22</v>
+        <v>121</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
       <c r="A58" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>20</v>
+        <v>125</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>25</v>
+        <v>127</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M58" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
       <c r="A59" s="1" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>124</v>
+        <v>37</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>125</v>
+        <v>20</v>
       </c>
       <c r="G59" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>126</v>
+        <v>22</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>19</v>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
+      <c r="A60" s="4" t="s">
+        <v>131</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="G60" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>22</v>
+        <v>114</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="L60" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
       <c r="A61" s="4" t="s">
         <v>131</v>
       </c>
+      <c r="B61" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E61" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="G61" s="3" t="s">
         <v>16</v>
@@ -2676,22 +2597,25 @@
       <c r="H61" s="1" t="s">
         <v>114</v>
       </c>
+      <c r="I61" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="K61" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
       <c r="A62" s="4" t="s">
         <v>131</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>21</v>
@@ -2703,94 +2627,95 @@
         <v>114</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>22</v>
+        <v>115</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+      <c r="L62" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
       <c r="A63" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>29</v>
+        <v>132</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G63" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>115</v>
+        <v>133</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>134</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L63" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13">
       <c r="A64" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="B64" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E64" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G64" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G64" s="7" t="s">
         <v>134</v>
       </c>
+      <c r="H64"/>
+      <c r="I64" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="K64" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
       <c r="A65" s="4" t="s">
         <v>132</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G65" s="8" t="s">
+      <c r="G65" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="H65" s="0"/>
+      <c r="H65"/>
       <c r="I65" s="1" t="s">
-        <v>22</v>
+        <v>135</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
       <c r="A66" s="4" t="s">
         <v>132</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>71</v>
+        <v>136</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>29</v>
@@ -2804,9 +2729,9 @@
       <c r="G66" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="H66" s="0"/>
+      <c r="H66"/>
       <c r="I66" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="K66" s="1" t="s">
         <v>25</v>
@@ -2815,136 +2740,97 @@
         <v>31</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:12">
       <c r="A67" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>29</v>
+        <v>138</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>21</v>
+        <v>139</v>
       </c>
       <c r="G67" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="H67" s="0"/>
-      <c r="I67" s="1" t="s">
-        <v>137</v>
-      </c>
+      <c r="H67"/>
       <c r="K67" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L67" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
       <c r="A68" s="4" t="s">
         <v>138</v>
       </c>
+      <c r="B68" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="E68" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>139</v>
+        <v>21</v>
       </c>
       <c r="G68" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="H68" s="0"/>
+      <c r="H68"/>
+      <c r="I68" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="K68" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G69" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="H69" s="0"/>
-      <c r="I69" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K69" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L69" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L68" s="1" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M35"/>
+  <autoFilter ref="A1:M34" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
-    <hyperlink ref="F44" r:id="rId1" display="http://snomed.info/sct"/>
-    <hyperlink ref="F45" r:id="rId2" display="http://snomed.info/sct"/>
-    <hyperlink ref="F46" r:id="rId3" display="http://snomed.info/sct"/>
-    <hyperlink ref="F47" r:id="rId4" display="http://snomed.info/sct"/>
-    <hyperlink ref="F48" r:id="rId5" display="http://snomed.info/sct"/>
-    <hyperlink ref="F49" r:id="rId6" display="http://snomed.info/sct"/>
-    <hyperlink ref="F50" r:id="rId7" display="http://snomed.info/sct"/>
-    <hyperlink ref="F55" r:id="rId8" display="http://snomed.info/sct"/>
-    <hyperlink ref="F56" r:id="rId9" display="http://snomed.info/sct"/>
+    <hyperlink ref="F43" r:id="rId1" display="http://snomed.info/sct" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F44" r:id="rId2" display="http://snomed.info/sct" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F45" r:id="rId3" display="http://snomed.info/sct" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F46" r:id="rId4" display="http://snomed.info/sct" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F47" r:id="rId5" display="http://snomed.info/sct" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F48" r:id="rId6" display="http://snomed.info/sct" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F49" r:id="rId7" display="http://snomed.info/sct" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F54" r:id="rId8" display="http://snomed.info/sct" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F55" r:id="rId9" display="http://snomed.info/sct" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId10"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="17.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="120.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="193.86"/>
+    <col min="1" max="1" width="37.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="17.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="120.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="69" style="1" customWidth="1"/>
+    <col min="13" max="13" width="193.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2985,7 +2871,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>119</v>
       </c>
@@ -3005,7 +2891,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>119</v>
       </c>
@@ -3031,7 +2917,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>84</v>
       </c>
@@ -3051,7 +2937,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>84</v>
       </c>
@@ -3077,7 +2963,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>84</v>
       </c>
@@ -3112,7 +2998,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
         <v>84</v>
       </c>
@@ -3144,7 +3030,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
         <v>84</v>
       </c>
@@ -3170,7 +3056,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
         <v>84</v>
       </c>
@@ -3196,7 +3082,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
         <v>84</v>
       </c>
@@ -3222,7 +3108,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
         <v>84</v>
       </c>
@@ -3245,7 +3131,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
         <v>84</v>
       </c>
@@ -3274,7 +3160,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
         <v>84</v>
       </c>
@@ -3306,7 +3192,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
         <v>84</v>
       </c>
@@ -3338,7 +3224,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:13">
       <c r="A15" s="1" t="s">
         <v>84</v>
       </c>
@@ -3364,7 +3250,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:13">
       <c r="A16" s="1" t="s">
         <v>84</v>
       </c>
@@ -3399,7 +3285,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
         <v>84</v>
       </c>
@@ -3422,7 +3308,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
         <v>84</v>
       </c>
@@ -3454,7 +3340,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:13">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -3474,7 +3360,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:13">
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
@@ -3500,7 +3386,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:13">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
@@ -3535,7 +3421,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:13">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
@@ -3564,7 +3450,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:13">
       <c r="A23" s="1" t="s">
         <v>131</v>
       </c>
@@ -3584,7 +3470,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:13">
       <c r="A24" s="1" t="s">
         <v>131</v>
       </c>
@@ -3610,7 +3496,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:13">
       <c r="A25" s="1" t="s">
         <v>131</v>
       </c>
@@ -3645,7 +3531,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:13">
       <c r="A26" s="1" t="s">
         <v>131</v>
       </c>
@@ -3671,7 +3557,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:13">
       <c r="A27" s="1" t="s">
         <v>13</v>
       </c>
@@ -3691,7 +3577,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:13" s="1" customFormat="1">
       <c r="A28" s="1" t="s">
         <v>13</v>
       </c>
@@ -3717,7 +3603,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:13">
       <c r="A29" s="1" t="s">
         <v>13</v>
       </c>
@@ -3749,7 +3635,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:13">
       <c r="A30" s="1" t="s">
         <v>13</v>
       </c>
@@ -3784,7 +3670,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:13">
       <c r="A31" s="1" t="s">
         <v>13</v>
       </c>
@@ -3813,7 +3699,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:13">
       <c r="A32" s="1" t="s">
         <v>39</v>
       </c>
@@ -3833,7 +3719,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:13">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -3859,7 +3745,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:13">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
@@ -3891,7 +3777,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:13">
       <c r="A35" s="1" t="s">
         <v>151</v>
       </c>
@@ -3911,7 +3797,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:13">
       <c r="A36" s="1" t="s">
         <v>151</v>
       </c>
@@ -3946,7 +3832,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:13">
       <c r="A37" s="1" t="s">
         <v>151</v>
       </c>
@@ -3981,7 +3867,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:13">
       <c r="A38" s="1" t="s">
         <v>155</v>
       </c>
@@ -4013,7 +3899,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:13">
       <c r="A39" s="1" t="s">
         <v>155</v>
       </c>
@@ -4048,7 +3934,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:13">
       <c r="A40" s="4" t="s">
         <v>68</v>
       </c>
@@ -4068,7 +3954,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:13">
       <c r="A41" s="4" t="s">
         <v>68</v>
       </c>
@@ -4094,7 +3980,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:13">
       <c r="A42" s="4" t="s">
         <v>68</v>
       </c>
@@ -4126,7 +4012,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:13">
       <c r="A43" s="4" t="s">
         <v>68</v>
       </c>
@@ -4164,7 +4050,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:13">
       <c r="A44" s="4" t="s">
         <v>68</v>
       </c>
@@ -4196,7 +4082,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:13">
       <c r="A45" s="4" t="s">
         <v>68</v>
       </c>
@@ -4235,13 +4121,8 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
@@ -4254,249 +4135,10 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A6BA5F8C2D628444819C98CC51374019" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d1ade1ff80079ef11d5f7598ff2bdcd2">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dab150e2-07c8-46cb-9249-a9bf8b457629" xmlns:ns4="3b2a6cf9-543e-463e-8642-d16a96cd5df5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="604d7b76327a76c6db5227909a871758" ns3:_="" ns4:_="">
-    <xsd:import namespace="dab150e2-07c8-46cb-9249-a9bf8b457629"/>
-    <xsd:import namespace="3b2a6cf9-543e-463e-8642-d16a96cd5df5"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns3:_activity" minOccurs="0"/>
-                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceSearchProperties" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceSystemTags" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="dab150e2-07c8-46cb-9249-a9bf8b457629" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="_activity" ma:index="8" nillable="true" ma:displayName="_activity" ma:hidden="true" ma:internalName="_activity">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceMetadata" ma:index="12" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="13" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="14" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="15" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSystemTags" ma:index="17" nillable="true" ma:displayName="MediaServiceSystemTags" ma:hidden="true" ma:internalName="MediaServiceSystemTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="18" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="19" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="21" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="3b2a6cf9-543e-463e-8642-d16a96cd5df5" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="9" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="10" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="SharingHintHash" ma:index="11" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="dab150e2-07c8-46cb-9249-a9bf8b457629" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A52368F7-EAC7-45FB-9A71-35E9ACE10DED}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE9DBFBC-8664-4C0E-9CBF-BAF1CF3B6304}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41D37996-5A98-4323-941F-5BAF649EAAF0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A52368F7-EAC7-45FB-9A71-35E9ACE10DED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update mapper dan format json
</commit_message>
<xml_diff>
--- a/Mapper.xlsx
+++ b/Mapper.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wulan Arief\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SafrialWiguna\source\repos\swrepo14461\ETL-FHIR-Beacon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA4EEFF-BBA7-497C-91E0-D8EAF1BBFA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEDDF5E-E54D-4677-86B6-FB2D3F3083F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapper" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="155">
   <si>
     <t>Where to Find</t>
   </si>
@@ -339,9 +339,6 @@
     <t>VALIDATE-NOT|component-array,code-object,coding-array,system-string|http://snomed.info/sct||COMBINED|GET-code-coding</t>
   </si>
   <si>
-    <t>VALIDATE-NOT|component-array,code-object,coding-array,system-string|http://snomed.info/sct||COMBINED|GET-valueCodeableConcept</t>
-  </si>
-  <si>
     <t>severity</t>
   </si>
   <si>
@@ -493,6 +490,12 @@
   </si>
   <si>
     <t>VALIDATE|clinicalStatus-object,coding-array,code-string|active||COMBINENEXT-1</t>
+  </si>
+  <si>
+    <t>VALIDATE-NOT|component-array,code-object,coding-array,system-string|http://snomed.info/sct||COMBINED|GET-valueCodeableConcept-coding</t>
+  </si>
+  <si>
+    <t>VALIDATE|component-array,code-object,coding-array,system-string|http://snomed.info/sct||COMBINED|GET-valueCodeableConcept-coding</t>
   </si>
 </sst>
 </file>
@@ -851,24 +854,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="62" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="F28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="37.453125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="27" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7265625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="17.54296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="185.81640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="17.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="185.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="25" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.54296875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="1" customWidth="1"/>
     <col min="10" max="10" width="17" style="1" customWidth="1"/>
-    <col min="11" max="11" width="19.54296875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" style="1" customWidth="1"/>
     <col min="12" max="12" width="69" style="1" customWidth="1"/>
-    <col min="13" max="13" width="193.81640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="193.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -1033,7 +1036,7 @@
         <v>14</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>16</v>
@@ -1296,7 +1299,7 @@
         <v>14</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>16</v>
@@ -1441,7 +1444,7 @@
         <v>14</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>16</v>
@@ -1659,7 +1662,7 @@
         <v>14</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>16</v>
@@ -1918,7 +1921,7 @@
         <v>14</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>16</v>
@@ -2002,7 +2005,7 @@
         <v>14</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>102</v>
+        <v>153</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>16</v>
@@ -2011,7 +2014,7 @@
         <v>17</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>25</v>
@@ -2031,7 +2034,7 @@
         <v>14</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>16</v>
@@ -2040,7 +2043,7 @@
         <v>17</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>43</v>
@@ -2057,7 +2060,7 @@
         <v>14</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>106</v>
+        <v>154</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>16</v>
@@ -2066,7 +2069,7 @@
         <v>36</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>25</v>
@@ -2087,7 +2090,7 @@
         <v>14</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>16</v>
@@ -2110,13 +2113,13 @@
         <v>14</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>25</v>
@@ -2142,10 +2145,10 @@
         <v>16</v>
       </c>
       <c r="H45" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I45" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>25</v>
@@ -2159,22 +2162,22 @@
         <v>82</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I46" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="K46" s="1" t="s">
         <v>20</v>
@@ -2185,7 +2188,7 @@
         <v>82</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>20</v>
@@ -2197,10 +2200,10 @@
         <v>16</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>20</v>
@@ -2211,11 +2214,11 @@
         <v>82</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="E48" s="1" t="s">
         <v>20</v>
       </c>
@@ -2226,10 +2229,10 @@
         <v>16</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>20</v>
@@ -2240,7 +2243,7 @@
         <v>82</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>20</v>
@@ -2252,7 +2255,7 @@
         <v>16</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>33</v>
@@ -2273,7 +2276,7 @@
         <v>14</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>16</v>
@@ -2282,7 +2285,7 @@
         <v>36</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>25</v>
@@ -2303,7 +2306,7 @@
         <v>14</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>16</v>
@@ -2320,7 +2323,7 @@
     </row>
     <row r="52" spans="1:13">
       <c r="A52" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>22</v>
@@ -2340,51 +2343,51 @@
     </row>
     <row r="53" spans="1:13">
       <c r="A53" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="E53" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H53" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E53" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H53" s="1" t="s">
+      <c r="K53" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L53" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="K53" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L53" s="1" t="s">
+      <c r="M53" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="M53" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:13">
       <c r="A54" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="G54" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H54" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G54" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H54" s="1" t="s">
+      <c r="K54" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="K54" s="1" t="s">
+      <c r="L54" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="L54" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="55" spans="1:13">
@@ -2407,27 +2410,27 @@
         <v>22</v>
       </c>
       <c r="K55" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L55" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="L55" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="56" spans="1:13">
       <c r="A56" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G56" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>25</v>
@@ -2435,7 +2438,7 @@
     </row>
     <row r="57" spans="1:13">
       <c r="A57" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>28</v>
@@ -2453,10 +2456,10 @@
         <v>16</v>
       </c>
       <c r="H57" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I57" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>25</v>
@@ -2467,10 +2470,10 @@
     </row>
     <row r="58" spans="1:13">
       <c r="A58" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>20</v>
@@ -2482,10 +2485,10 @@
         <v>16</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K58" s="1" t="s">
         <v>20</v>
@@ -2493,14 +2496,14 @@
     </row>
     <row r="59" spans="1:13">
       <c r="A59" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="E59" s="1" t="s">
         <v>20</v>
       </c>
@@ -2511,10 +2514,10 @@
         <v>16</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>20</v>
@@ -2565,7 +2568,7 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
@@ -2613,20 +2616,20 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="37.453125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="27" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7265625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="17.54296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="120.453125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="17.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="120.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="25" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.54296875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="1" customWidth="1"/>
     <col min="10" max="10" width="17" style="1" customWidth="1"/>
-    <col min="11" max="11" width="19.54296875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" style="1" customWidth="1"/>
     <col min="12" max="12" width="69" style="1" customWidth="1"/>
-    <col min="13" max="13" width="193.81640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="193.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -2672,7 +2675,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>22</v>
@@ -2692,28 +2695,28 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="K3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -2724,7 +2727,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>16</v>
@@ -2834,7 +2837,7 @@
         <v>82</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>43</v>
@@ -2860,10 +2863,10 @@
         <v>82</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>21</v>
@@ -2878,7 +2881,7 @@
         <v>85</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -2886,7 +2889,7 @@
         <v>82</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>20</v>
@@ -2918,7 +2921,7 @@
         <v>14</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>16</v>
@@ -2938,13 +2941,13 @@
         <v>89</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>16</v>
@@ -2953,7 +2956,7 @@
         <v>17</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>43</v>
@@ -3002,7 +3005,7 @@
         <v>14</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>16</v>
@@ -3011,7 +3014,7 @@
         <v>17</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>25</v>
@@ -3034,7 +3037,7 @@
         <v>14</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>16</v>
@@ -3095,7 +3098,7 @@
         <v>14</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>16</v>
@@ -3251,19 +3254,19 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>14</v>
@@ -3271,7 +3274,7 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>22</v>
@@ -3286,7 +3289,7 @@
         <v>16</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>22</v>
@@ -3297,7 +3300,7 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>28</v>
@@ -3315,10 +3318,10 @@
         <v>16</v>
       </c>
       <c r="H25" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>25</v>
@@ -3332,10 +3335,10 @@
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>20</v>
@@ -3347,10 +3350,10 @@
         <v>16</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>20</v>
@@ -3428,7 +3431,7 @@
         <v>25</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M29" s="1" t="s">
         <v>27</v>
@@ -3578,13 +3581,13 @@
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>16</v>
@@ -3598,7 +3601,7 @@
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>66</v>
@@ -3633,10 +3636,10 @@
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>19</v>
@@ -3645,7 +3648,7 @@
         <v>25</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>16</v>
@@ -3668,7 +3671,7 @@
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>56</v>
@@ -3700,7 +3703,7 @@
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>56</v>
@@ -3741,7 +3744,7 @@
         <v>14</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>16</v>
@@ -3787,7 +3790,7 @@
         <v>68</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>14</v>
@@ -3933,11 +3936,11 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update mapper dan validasi
</commit_message>
<xml_diff>
--- a/Mapper.xlsx
+++ b/Mapper.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SafrialWiguna\source\repos\swrepo14461\ETL-FHIR-Beacon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:41000001_{CBB6DFA4-DFAF-3244-A24F-2C25653248F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A37658-B7FD-4256-B205-5DA068278E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="156">
   <si>
     <t>Where to Find</t>
   </si>
@@ -507,13 +507,16 @@
   </si>
   <si>
     <t>VALIDATE|component-array,code-object,coding-array,system-string|http://snomed.info/sct||COMBINED|GET-valueCodeableConcept-coding</t>
+  </si>
+  <si>
+    <t>COMBINED|GETVALID-system,http://hl7.org/fhir/sid/icd%2D9%2Dcm;http://hl7.org/fhir/sid/icd%2D10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -865,27 +868,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.609375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="37.39453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.0390625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7734375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="17.62109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="185.91015625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.31640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="25.01953125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.5234375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.94921875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="19.50390625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="69.0078125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="193.84765625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="17.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="185.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="69" style="1" customWidth="1"/>
+    <col min="13" max="13" width="193.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="15" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -926,7 +929,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -946,7 +949,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="15" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -978,7 +981,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="15" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1010,7 +1013,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1039,7 +1042,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="15" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -1059,7 +1062,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="15" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
@@ -1073,7 +1076,7 @@
         <v>14</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>21</v>
+        <v>155</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>16</v>
@@ -1091,7 +1094,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="15" customHeight="1">
       <c r="A8" s="4" t="s">
         <v>39</v>
       </c>
@@ -1111,7 +1114,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="15" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>39</v>
       </c>
@@ -1140,7 +1143,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
@@ -1169,7 +1172,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="15" customHeight="1">
       <c r="A11" s="4" t="s">
         <v>47</v>
       </c>
@@ -1189,7 +1192,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="15" customHeight="1">
       <c r="A12" s="4" t="s">
         <v>47</v>
       </c>
@@ -1218,7 +1221,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="15" customHeight="1">
       <c r="A13" s="4" t="s">
         <v>47</v>
       </c>
@@ -1250,7 +1253,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="15" customHeight="1">
       <c r="A14" s="4" t="s">
         <v>51</v>
       </c>
@@ -1270,7 +1273,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="15" customHeight="1">
       <c r="A15" s="4" t="s">
         <v>51</v>
       </c>
@@ -1302,7 +1305,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="15" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>55</v>
       </c>
@@ -1322,7 +1325,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="15" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>55</v>
       </c>
@@ -1351,7 +1354,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="15" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>55</v>
       </c>
@@ -1383,7 +1386,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="15" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
@@ -1415,7 +1418,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="15" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>55</v>
       </c>
@@ -1447,7 +1450,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="15" customHeight="1">
       <c r="A21" s="4" t="s">
         <v>67</v>
       </c>
@@ -1467,7 +1470,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="15" customHeight="1">
       <c r="A22" s="4" t="s">
         <v>67</v>
       </c>
@@ -1499,7 +1502,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="15" customHeight="1">
       <c r="A23" s="4" t="s">
         <v>67</v>
       </c>
@@ -1531,7 +1534,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1">
       <c r="A24" s="4" t="s">
         <v>67</v>
       </c>
@@ -1563,7 +1566,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="15" customHeight="1">
       <c r="A25" s="4" t="s">
         <v>67</v>
       </c>
@@ -1598,7 +1601,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="15" customHeight="1">
       <c r="A26" s="4" t="s">
         <v>67</v>
       </c>
@@ -1630,7 +1633,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="15" customHeight="1">
       <c r="A27" s="4" t="s">
         <v>67</v>
       </c>
@@ -1665,7 +1668,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="A28" s="4" t="s">
         <v>82</v>
       </c>
@@ -1685,7 +1688,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13">
       <c r="A29" s="1" t="s">
         <v>82</v>
       </c>
@@ -1717,7 +1720,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="A30" s="1" t="s">
         <v>82</v>
       </c>
@@ -1749,7 +1752,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13">
       <c r="A31" s="1" t="s">
         <v>82</v>
       </c>
@@ -1775,7 +1778,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="A32" s="1" t="s">
         <v>82</v>
       </c>
@@ -1804,7 +1807,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12">
       <c r="A33" s="1" t="s">
         <v>82</v>
       </c>
@@ -1833,7 +1836,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12">
       <c r="A34" s="1" t="s">
         <v>82</v>
       </c>
@@ -1859,7 +1862,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12">
       <c r="A35" s="1" t="s">
         <v>82</v>
       </c>
@@ -1891,7 +1894,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12">
       <c r="A36" s="1" t="s">
         <v>82</v>
       </c>
@@ -1924,7 +1927,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12">
       <c r="A37" s="4" t="s">
         <v>82</v>
       </c>
@@ -1944,7 +1947,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12">
       <c r="A38" s="1" t="s">
         <v>82</v>
       </c>
@@ -1976,7 +1979,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12">
       <c r="A39" s="1" t="s">
         <v>82</v>
       </c>
@@ -2005,7 +2008,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12">
       <c r="A40" s="1" t="s">
         <v>82</v>
       </c>
@@ -2034,7 +2037,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12">
       <c r="A41" s="1" t="s">
         <v>82</v>
       </c>
@@ -2060,7 +2063,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12">
       <c r="A42" s="1" t="s">
         <v>82</v>
       </c>
@@ -2089,7 +2092,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12">
       <c r="A43" s="1" t="s">
         <v>82</v>
       </c>
@@ -2116,7 +2119,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12">
       <c r="A44" s="4" t="s">
         <v>82</v>
       </c>
@@ -2136,7 +2139,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12">
       <c r="A45" s="4" t="s">
         <v>82</v>
       </c>
@@ -2168,7 +2171,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12">
       <c r="A46" s="1" t="s">
         <v>82</v>
       </c>
@@ -2194,7 +2197,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12">
       <c r="A47" s="1" t="s">
         <v>82</v>
       </c>
@@ -2220,7 +2223,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12">
       <c r="A48" s="1" t="s">
         <v>82</v>
       </c>
@@ -2249,7 +2252,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13">
       <c r="A49" s="1" t="s">
         <v>82</v>
       </c>
@@ -2275,7 +2278,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13">
       <c r="A50" s="1" t="s">
         <v>82</v>
       </c>
@@ -2305,7 +2308,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13">
       <c r="A51" s="1" t="s">
         <v>82</v>
       </c>
@@ -2332,7 +2335,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13">
       <c r="A52" s="1" t="s">
         <v>113</v>
       </c>
@@ -2352,7 +2355,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13">
       <c r="A53" s="1" t="s">
         <v>113</v>
       </c>
@@ -2378,7 +2381,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13">
       <c r="A54" s="1" t="s">
         <v>113</v>
       </c>
@@ -2401,7 +2404,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13">
       <c r="A55" s="1" t="s">
         <v>82</v>
       </c>
@@ -2427,7 +2430,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13">
       <c r="A56" s="4" t="s">
         <v>125</v>
       </c>
@@ -2447,7 +2450,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13">
       <c r="A57" s="4" t="s">
         <v>125</v>
       </c>
@@ -2479,7 +2482,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13">
       <c r="A58" s="4" t="s">
         <v>125</v>
       </c>
@@ -2505,7 +2508,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13">
       <c r="A59" s="4" t="s">
         <v>125</v>
       </c>
@@ -2534,22 +2537,22 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13">
       <c r="A60" s="4"/>
       <c r="G60" s="5"/>
       <c r="H60"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13">
       <c r="A61" s="4"/>
       <c r="G61" s="5"/>
       <c r="H61"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13">
       <c r="A62" s="4"/>
       <c r="G62" s="5"/>
       <c r="H62"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13">
       <c r="A63" s="4"/>
       <c r="G63" s="5"/>
       <c r="H63"/>
@@ -2579,9 +2582,9 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -2627,23 +2630,23 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.609375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="37.39453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.0390625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7734375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="17.62109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="120.3984375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.31640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="25.01953125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.5234375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.94921875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="19.50390625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="69.0078125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="193.84765625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="17.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="120.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="69" style="1" customWidth="1"/>
+    <col min="13" max="13" width="193.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="15" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2684,7 +2687,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>113</v>
       </c>
@@ -2704,7 +2707,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="15" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>113</v>
       </c>
@@ -2730,7 +2733,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="15" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>82</v>
       </c>
@@ -2750,7 +2753,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>82</v>
       </c>
@@ -2776,7 +2779,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="15" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>82</v>
       </c>
@@ -2811,7 +2814,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="15" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>82</v>
       </c>
@@ -2843,7 +2846,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="15" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>82</v>
       </c>
@@ -2869,7 +2872,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="15" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>82</v>
       </c>
@@ -2895,7 +2898,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>82</v>
       </c>
@@ -2921,7 +2924,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="15" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>82</v>
       </c>
@@ -2944,7 +2947,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="15" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>82</v>
       </c>
@@ -2973,7 +2976,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="15" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>82</v>
       </c>
@@ -3005,7 +3008,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="15" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>82</v>
       </c>
@@ -3037,7 +3040,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="15" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>82</v>
       </c>
@@ -3063,7 +3066,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="15" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>82</v>
       </c>
@@ -3098,7 +3101,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="15" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>82</v>
       </c>
@@ -3121,7 +3124,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="15" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>82</v>
       </c>
@@ -3153,7 +3156,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="15" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -3173,7 +3176,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="15" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
@@ -3199,7 +3202,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="15" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
@@ -3234,7 +3237,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="15" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
@@ -3263,7 +3266,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="15" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>125</v>
       </c>
@@ -3283,7 +3286,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="15" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>125</v>
       </c>
@@ -3309,7 +3312,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="15" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>125</v>
       </c>
@@ -3344,7 +3347,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="15" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>125</v>
       </c>
@@ -3370,7 +3373,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="15" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>13</v>
       </c>
@@ -3390,7 +3393,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>13</v>
       </c>
@@ -3416,7 +3419,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="15" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>13</v>
       </c>
@@ -3448,7 +3451,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="15" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>13</v>
       </c>
@@ -3483,7 +3486,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="15" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>13</v>
       </c>
@@ -3512,7 +3515,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="15" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>39</v>
       </c>
@@ -3532,7 +3535,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="15" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -3558,7 +3561,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="15" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>39</v>
       </c>
@@ -3590,7 +3593,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" ht="15" customHeight="1">
       <c r="A35" s="1" t="s">
         <v>137</v>
       </c>
@@ -3610,7 +3613,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13">
       <c r="A36" s="1" t="s">
         <v>137</v>
       </c>
@@ -3645,7 +3648,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13">
       <c r="A37" s="1" t="s">
         <v>137</v>
       </c>
@@ -3680,7 +3683,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13">
       <c r="A38" s="1" t="s">
         <v>141</v>
       </c>
@@ -3712,7 +3715,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13">
       <c r="A39" s="1" t="s">
         <v>141</v>
       </c>
@@ -3747,7 +3750,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13">
       <c r="A40" s="4" t="s">
         <v>67</v>
       </c>
@@ -3767,7 +3770,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13">
       <c r="A41" s="4" t="s">
         <v>67</v>
       </c>
@@ -3793,7 +3796,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13">
       <c r="A42" s="4" t="s">
         <v>67</v>
       </c>
@@ -3825,7 +3828,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13">
       <c r="A43" s="4" t="s">
         <v>67</v>
       </c>
@@ -3863,7 +3866,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13">
       <c r="A44" s="4" t="s">
         <v>67</v>
       </c>
@@ -3895,7 +3898,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13">
       <c r="A45" s="4" t="s">
         <v>67</v>
       </c>
@@ -3947,9 +3950,9 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>150</v>
       </c>

</xml_diff>

<commit_message>
update mapper fix header
</commit_message>
<xml_diff>
--- a/Mapper.xlsx
+++ b/Mapper.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wulan Arief\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SafrialWiguna\source\repos\swrepo14461\ETL-FHIR-Beacon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027AF7FE-ABE3-404B-8B36-CDD2C90EDBC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C42023A-5936-4614-A3BE-685BAD401A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapper" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Mapper!$A$1:$M$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Mapper!$A$1:$M$60</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="157">
   <si>
     <t>Where to Find</t>
   </si>
@@ -499,6 +499,9 @@
   </si>
   <si>
     <t>VALIDATE|status-string|completedORfinal||VALIDATE|category-array,coding-array,code-string|examORimaging||VALIDATE-HAD|component-array||COMBINENEXT-4</t>
+  </si>
+  <si>
+    <t>VALIDATE|status-string|completedORfinal||VALIDATE|category-array,coding-array,code-string|examORimaging||VALIDATE-HAD|component-array||COMBINENEXT-2</t>
   </si>
 </sst>
 </file>
@@ -855,26 +858,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M63"/>
+  <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="37.453125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="27" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7265625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="17.54296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="185.81640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="17.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="185.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="25" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.54296875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="1" customWidth="1"/>
     <col min="10" max="10" width="17" style="1" customWidth="1"/>
-    <col min="11" max="11" width="19.54296875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="88.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="193.81640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="88.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="193.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1">
@@ -1657,7 +1660,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="14.5">
+    <row r="28" spans="1:13">
       <c r="A28" s="4" t="s">
         <v>82</v>
       </c>
@@ -1677,7 +1680,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="14.5">
+    <row r="29" spans="1:13">
       <c r="A29" s="1" t="s">
         <v>82</v>
       </c>
@@ -1709,7 +1712,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="14.5">
+    <row r="30" spans="1:13">
       <c r="A30" s="1" t="s">
         <v>82</v>
       </c>
@@ -1741,7 +1744,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="14.5">
+    <row r="31" spans="1:13">
       <c r="A31" s="1" t="s">
         <v>82</v>
       </c>
@@ -1767,7 +1770,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="14.5">
+    <row r="32" spans="1:13">
       <c r="A32" s="1" t="s">
         <v>82</v>
       </c>
@@ -1796,7 +1799,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="14.5">
+    <row r="33" spans="1:12">
       <c r="A33" s="1" t="s">
         <v>82</v>
       </c>
@@ -1825,7 +1828,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="14.5">
+    <row r="34" spans="1:12">
       <c r="A34" s="1" t="s">
         <v>82</v>
       </c>
@@ -1851,7 +1854,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="14.5">
+    <row r="35" spans="1:12">
       <c r="A35" s="1" t="s">
         <v>82</v>
       </c>
@@ -1883,7 +1886,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="14.5">
+    <row r="36" spans="1:12">
       <c r="A36" s="1" t="s">
         <v>82</v>
       </c>
@@ -1916,7 +1919,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="14.5">
+    <row r="37" spans="1:12">
       <c r="A37" s="4" t="s">
         <v>82</v>
       </c>
@@ -1936,7 +1939,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="14.5">
+    <row r="38" spans="1:12">
       <c r="A38" s="1" t="s">
         <v>82</v>
       </c>
@@ -1968,7 +1971,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="14.5">
+    <row r="39" spans="1:12">
       <c r="A39" s="1" t="s">
         <v>82</v>
       </c>
@@ -1997,7 +2000,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="14.5">
+    <row r="40" spans="1:12">
       <c r="A40" s="1" t="s">
         <v>82</v>
       </c>
@@ -2026,7 +2029,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="14.5">
+    <row r="41" spans="1:12">
       <c r="A41" s="1" t="s">
         <v>82</v>
       </c>
@@ -2052,18 +2055,15 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="14" customHeight="1">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:12">
+      <c r="A42" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="E42" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>16</v>
@@ -2071,29 +2071,22 @@
       <c r="H42" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I42" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="K42" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="14.5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="14.1" customHeight="1">
       <c r="A43" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C43"/>
       <c r="E43" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>107</v>
+        <v>153</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>16</v>
@@ -2102,47 +2095,51 @@
         <v>36</v>
       </c>
       <c r="I43" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44"/>
+      <c r="E44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I44" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K43" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="14.5">
-      <c r="A44" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="K44" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="14.5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
       <c r="A45" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="E45" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>21</v>
+        <v>144</v>
       </c>
       <c r="G45" s="3" t="s">
         <v>16</v>
@@ -2150,25 +2147,22 @@
       <c r="H45" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="I45" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="K45" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L45" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="14.5">
-      <c r="A46" s="1" t="s">
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="4" t="s">
         <v>82</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>110</v>
+        <v>28</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>21</v>
@@ -2180,18 +2174,21 @@
         <v>108</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="14.5">
+        <v>25</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
       <c r="A47" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>20</v>
@@ -2212,15 +2209,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="14.5">
+    <row r="48" spans="1:12">
       <c r="A48" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>20</v>
@@ -2241,12 +2235,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="14.5">
+    <row r="49" spans="1:13">
       <c r="A49" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>112</v>
+        <v>145</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>146</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>20</v>
@@ -2261,43 +2258,39 @@
         <v>108</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>33</v>
+        <v>111</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="14.5">
+    <row r="50" spans="1:13">
       <c r="A50" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C50"/>
+        <v>112</v>
+      </c>
       <c r="E50" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>105</v>
+        <v>21</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>36</v>
+        <v>108</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L50" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" ht="14.5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
       <c r="A51" s="1" t="s">
         <v>82</v>
       </c>
@@ -2309,7 +2302,7 @@
         <v>14</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>16</v>
@@ -2318,38 +2311,48 @@
         <v>36</v>
       </c>
       <c r="I51" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52"/>
+      <c r="E52" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I52" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K51" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" ht="14.5">
-      <c r="A52" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="K52" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="14.5">
+    <row r="53" spans="1:13">
       <c r="A53" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>114</v>
+        <v>22</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>20</v>
@@ -2358,102 +2361,96 @@
         <v>16</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>115</v>
+        <v>22</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L53" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="M53" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" ht="14.5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
       <c r="A54" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="E55" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G54" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H54" s="1" t="s">
+      <c r="G55" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H55" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="K54" s="1" t="s">
+      <c r="K55" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="L54" s="1" t="s">
+      <c r="L55" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="14.5">
-      <c r="A55" s="1" t="s">
+    <row r="56" spans="1:13">
+      <c r="A56" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H55" s="1" t="s">
+      <c r="E56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H56" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K55" s="1" t="s">
+      <c r="K56" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="L55" s="1" t="s">
+      <c r="L56" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="14.5">
-      <c r="A56" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" ht="14.5">
+    <row r="57" spans="1:13">
       <c r="A57" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="E57" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>21</v>
+        <v>134</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>16</v>
@@ -2461,25 +2458,22 @@
       <c r="H57" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="I57" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="K57" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L57" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" ht="14.5">
+    </row>
+    <row r="58" spans="1:13">
       <c r="A58" s="4" t="s">
         <v>125</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>135</v>
+        <v>28</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>21</v>
@@ -2491,21 +2485,21 @@
         <v>108</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" ht="14.5">
+        <v>25</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
       <c r="A59" s="4" t="s">
         <v>125</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>20</v>
@@ -2526,25 +2520,54 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="14.5">
-      <c r="A60" s="4"/>
-      <c r="G60" s="5"/>
-      <c r="H60"/>
-    </row>
-    <row r="61" spans="1:13" ht="14.5">
+    <row r="60" spans="1:13">
+      <c r="A60" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
       <c r="A61" s="4"/>
       <c r="G61" s="5"/>
       <c r="H61"/>
     </row>
-    <row r="62" spans="1:13" ht="14.5">
+    <row r="62" spans="1:13">
       <c r="A62" s="4"/>
       <c r="G62" s="5"/>
       <c r="H62"/>
     </row>
-    <row r="63" spans="1:13" ht="14.5">
+    <row r="63" spans="1:13">
       <c r="A63" s="4"/>
       <c r="G63" s="5"/>
       <c r="H63"/>
+    </row>
+    <row r="64" spans="1:13">
+      <c r="A64" s="4"/>
+      <c r="G64" s="5"/>
+      <c r="H64"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2552,10 +2575,10 @@
     <hyperlink ref="F39" r:id="rId2" display="http://snomed.info/sct" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="F40" r:id="rId3" display="http://snomed.info/sct" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="F41" r:id="rId4" display="http://snomed.info/sct" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="F42" r:id="rId5" display="http://snomed.info/sct" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="F43" r:id="rId6" display="http://snomed.info/sct" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="F50" r:id="rId7" display="http://snomed.info/sct" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="F51" r:id="rId8" display="http://snomed.info/sct" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F43" r:id="rId5" display="http://snomed.info/sct" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F44" r:id="rId6" display="http://snomed.info/sct" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F51" r:id="rId7" display="http://snomed.info/sct" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F52" r:id="rId8" display="http://snomed.info/sct" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2570,17 +2593,17 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="104.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="104.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="50" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2632,20 +2655,20 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="37.453125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="27" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7265625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="17.54296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="120.453125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="17.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="120.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="25" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.54296875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="1" customWidth="1"/>
     <col min="10" max="10" width="17" style="1" customWidth="1"/>
-    <col min="11" max="11" width="19.54296875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" style="1" customWidth="1"/>
     <col min="12" max="12" width="69" style="1" customWidth="1"/>
-    <col min="13" max="13" width="193.81640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="193.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1">
@@ -3615,7 +3638,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="14.5">
+    <row r="36" spans="1:13">
       <c r="A36" s="1" t="s">
         <v>137</v>
       </c>
@@ -3650,7 +3673,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="14.5">
+    <row r="37" spans="1:13">
       <c r="A37" s="1" t="s">
         <v>137</v>
       </c>
@@ -3685,7 +3708,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="14.5">
+    <row r="38" spans="1:13">
       <c r="A38" s="1" t="s">
         <v>141</v>
       </c>
@@ -3717,7 +3740,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="14.5">
+    <row r="39" spans="1:13">
       <c r="A39" s="1" t="s">
         <v>141</v>
       </c>
@@ -3752,7 +3775,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="14.5">
+    <row r="40" spans="1:13">
       <c r="A40" s="4" t="s">
         <v>67</v>
       </c>
@@ -3772,7 +3795,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="14.5">
+    <row r="41" spans="1:13">
       <c r="A41" s="4" t="s">
         <v>67</v>
       </c>
@@ -3798,7 +3821,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="14.5">
+    <row r="42" spans="1:13">
       <c r="A42" s="4" t="s">
         <v>67</v>
       </c>
@@ -3830,7 +3853,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="14.5">
+    <row r="43" spans="1:13">
       <c r="A43" s="4" t="s">
         <v>67</v>
       </c>
@@ -3868,7 +3891,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="14.5">
+    <row r="44" spans="1:13">
       <c r="A44" s="4" t="s">
         <v>67</v>
       </c>
@@ -3900,7 +3923,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="14.5">
+    <row r="45" spans="1:13">
       <c r="A45" s="4" t="s">
         <v>67</v>
       </c>
@@ -3952,7 +3975,7 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">

</xml_diff>